<commit_message>
added 6 params regression
</commit_message>
<xml_diff>
--- a/protein_Belgorod.xlsx
+++ b/protein_Belgorod.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkd\dev\diploma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712B68EB-BFFF-4A13-9FBD-EBFE57C4D72D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189E4F2E-50C7-4E43-BC87-8D4BF3AB808F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2475" yWindow="1440" windowWidth="21600" windowHeight="11385" xr2:uid="{4ADC32DF-F1DC-4277-9E07-398DF3F93614}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4ADC32DF-F1DC-4277-9E07-398DF3F93614}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист2" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>year</t>
   </si>
@@ -135,6 +135,54 @@
   </si>
   <si>
     <t>protein_full</t>
+  </si>
+  <si>
+    <t>E_v</t>
+  </si>
+  <si>
+    <t>Pss_v</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.203333333333333</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3.67</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5.513333333333333</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5.346666666666667</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.296666666666667</t>
+  </si>
+  <si>
+    <t>Ob_v</t>
+  </si>
+  <si>
+    <t>HTC_v</t>
+  </si>
+  <si>
+    <t>R_v_full</t>
+  </si>
+  <si>
+    <t>T_v_full</t>
+  </si>
+  <si>
+    <t>E_v_full</t>
+  </si>
+  <si>
+    <t>Pss_v_full</t>
+  </si>
+  <si>
+    <t>Ob_v_full</t>
+  </si>
+  <si>
+    <t>HTC_v_full</t>
+  </si>
+  <si>
+    <t>protein_forecast</t>
   </si>
 </sst>
 </file>
@@ -1312,6 +1360,484 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.1039370078740162E-2"/>
+          <c:y val="5.0925925925925923E-2"/>
+          <c:w val="0.88396062992125979"/>
+          <c:h val="0.73577136191309422"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>full!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>protein_forecast</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>full!$I$2:$I$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>11.21113487</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.479931669999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.31141117</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.47833582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.476951509999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.436777230000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.038451540000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.5054663</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.84617278</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.859356460000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.81090605</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.40419234</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.980670249999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.4879038100000006</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11.972047160000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.57489485</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12.908599499999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12.529942569999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12.966400200000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12.04823423</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13.898573499999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12.848453109999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13.89854016</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12.9389074</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11.83763589</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11.98232353</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13.413161710000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>12.67487704</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14.218488450000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>12.937180870000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>12.493339020000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>12.2148875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D474-4E82-9824-23BE64ACEB97}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>full!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>protein_full</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>full!$J$2:$J$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="1">
+                  <c:v>9.163636363636364</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.660869565217391</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.877777777777776</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.562068965517241</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.473333333333333</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.314285714285713</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.642857142857142</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.31891891891892</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.135</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.588888888888889</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12.28</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12.725</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13.112500000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13.309090909090909</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11.176923076923078</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15.042857142857141</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12.532142857142857</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>14.05</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12.37142857142857</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14.416666666666666</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>12.55</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>12.01</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>12.753846153846153</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D474-4E82-9824-23BE64ACEB97}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1507562959"/>
+        <c:axId val="1417972623"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1507562959"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1417972623"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1417972623"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1507562959"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:title>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2008,6 +2534,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2525,7 +3091,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2552,8 +3118,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2633,6 +3199,522 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -3044,16 +4126,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>438149</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>390524</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3082,6 +4164,47 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE5ACAF2-70F9-4EF7-B195-456FA298F22F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3419,10 +4542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{139D87CC-99BC-47AF-8614-82F5A31FEE7F}">
-  <dimension ref="A1:Z28"/>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3435,6 +4558,10 @@
     <col min="9" max="10" width="19" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -3474,6 +4601,42 @@
       <c r="L1" t="s">
         <v>33</v>
       </c>
+      <c r="M1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -3512,6 +4675,42 @@
       <c r="L2" s="2">
         <v>9.163636363636364</v>
       </c>
+      <c r="M2">
+        <v>33.099999999999902</v>
+      </c>
+      <c r="N2">
+        <v>992</v>
+      </c>
+      <c r="O2" s="1">
+        <v>6.1666666666666599</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1.26383634580355</v>
+      </c>
+      <c r="Q2">
+        <v>267.8</v>
+      </c>
+      <c r="R2">
+        <v>300</v>
+      </c>
+      <c r="S2">
+        <v>33.4</v>
+      </c>
+      <c r="T2">
+        <v>821</v>
+      </c>
+      <c r="U2" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="V2" s="1">
+        <v>0.88983473547700498</v>
+      </c>
+      <c r="W2" s="2">
+        <v>10.479931669999999</v>
+      </c>
+      <c r="X2" s="2">
+        <v>9.163636363636364</v>
+      </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -3550,6 +4749,42 @@
       <c r="L3" s="2">
         <v>11.660869565217391</v>
       </c>
+      <c r="M3">
+        <v>46.9</v>
+      </c>
+      <c r="N3">
+        <v>901</v>
+      </c>
+      <c r="O3" s="1">
+        <v>4.6666666666666599</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0.86507189671966001</v>
+      </c>
+      <c r="Q3">
+        <v>360.8</v>
+      </c>
+      <c r="R3">
+        <v>285</v>
+      </c>
+      <c r="S3">
+        <v>33.099999999999902</v>
+      </c>
+      <c r="T3">
+        <v>992</v>
+      </c>
+      <c r="U3" s="1">
+        <v>6.1666666666666599</v>
+      </c>
+      <c r="V3" s="1">
+        <v>1.26383634580355</v>
+      </c>
+      <c r="W3" s="2">
+        <v>13.31141117</v>
+      </c>
+      <c r="X3" s="2">
+        <v>11.660869565217391</v>
+      </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -3588,6 +4823,42 @@
       <c r="L4" s="2">
         <v>10.877777777777776</v>
       </c>
+      <c r="M4">
+        <v>42.199999999999903</v>
+      </c>
+      <c r="N4">
+        <v>1022</v>
+      </c>
+      <c r="O4" s="1">
+        <v>5.1999999999999904</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0.59789761003428099</v>
+      </c>
+      <c r="Q4">
+        <v>262</v>
+      </c>
+      <c r="R4">
+        <v>302</v>
+      </c>
+      <c r="S4">
+        <v>46.9</v>
+      </c>
+      <c r="T4">
+        <v>901</v>
+      </c>
+      <c r="U4" s="1">
+        <v>4.6666666666666599</v>
+      </c>
+      <c r="V4" s="1">
+        <v>0.86507189671966001</v>
+      </c>
+      <c r="W4" s="2">
+        <v>10.476951509999999</v>
+      </c>
+      <c r="X4" s="2">
+        <v>10.877777777777776</v>
+      </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -3626,6 +4897,42 @@
       <c r="L5" s="2">
         <v>11.562068965517241</v>
       </c>
+      <c r="M5">
+        <v>36.9</v>
+      </c>
+      <c r="N5">
+        <v>908</v>
+      </c>
+      <c r="O5" s="1">
+        <v>4.6533333333333298</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0.85631224949684304</v>
+      </c>
+      <c r="Q5">
+        <v>385.8</v>
+      </c>
+      <c r="R5">
+        <v>295</v>
+      </c>
+      <c r="S5">
+        <v>41.3</v>
+      </c>
+      <c r="T5">
+        <v>941</v>
+      </c>
+      <c r="U5" s="1">
+        <v>5.6666666666666599</v>
+      </c>
+      <c r="V5" s="1">
+        <v>1.30808483225117</v>
+      </c>
+      <c r="W5" s="2">
+        <v>12.038451540000001</v>
+      </c>
+      <c r="X5" s="2">
+        <v>11.562068965517241</v>
+      </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -3664,6 +4971,42 @@
       <c r="L6" s="2">
         <v>13.473333333333333</v>
       </c>
+      <c r="M6">
+        <v>44.5</v>
+      </c>
+      <c r="N6">
+        <v>860</v>
+      </c>
+      <c r="O6" s="1">
+        <v>5.4866666666666601</v>
+      </c>
+      <c r="P6" s="1">
+        <v>1.3037883725205099</v>
+      </c>
+      <c r="Q6">
+        <v>184</v>
+      </c>
+      <c r="R6">
+        <v>307</v>
+      </c>
+      <c r="S6">
+        <v>42.199999999999903</v>
+      </c>
+      <c r="T6">
+        <v>1022</v>
+      </c>
+      <c r="U6" s="1">
+        <v>5.1999999999999904</v>
+      </c>
+      <c r="V6" s="1">
+        <v>0.59789761003428099</v>
+      </c>
+      <c r="W6" s="2">
+        <v>13.5054663</v>
+      </c>
+      <c r="X6" s="2">
+        <v>13.473333333333333</v>
+      </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -3702,6 +5045,42 @@
       <c r="L7" s="2">
         <v>12.314285714285713</v>
       </c>
+      <c r="M7">
+        <v>41.3</v>
+      </c>
+      <c r="N7">
+        <v>957</v>
+      </c>
+      <c r="O7" s="1">
+        <v>3.91333333333333</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0.93909346089325096</v>
+      </c>
+      <c r="Q7">
+        <v>280.2</v>
+      </c>
+      <c r="R7">
+        <v>315</v>
+      </c>
+      <c r="S7">
+        <v>41.7</v>
+      </c>
+      <c r="T7">
+        <v>931</v>
+      </c>
+      <c r="U7" s="1">
+        <v>6.1999999999999904</v>
+      </c>
+      <c r="V7" s="1">
+        <v>0.88934029485979005</v>
+      </c>
+      <c r="W7" s="2">
+        <v>12.84617278</v>
+      </c>
+      <c r="X7" s="2">
+        <v>12.314285714285713</v>
+      </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -3740,6 +5119,42 @@
       <c r="L8" s="2">
         <v>10.642857142857142</v>
       </c>
+      <c r="M8">
+        <v>40</v>
+      </c>
+      <c r="N8">
+        <v>967</v>
+      </c>
+      <c r="O8" s="1">
+        <v>5.17</v>
+      </c>
+      <c r="P8" s="1">
+        <v>1.0463899546564299</v>
+      </c>
+      <c r="Q8">
+        <v>248.9</v>
+      </c>
+      <c r="R8">
+        <v>290</v>
+      </c>
+      <c r="S8">
+        <v>36.9</v>
+      </c>
+      <c r="T8">
+        <v>908</v>
+      </c>
+      <c r="U8" s="1">
+        <v>4.6533333333333298</v>
+      </c>
+      <c r="V8" s="1">
+        <v>0.85631224949684304</v>
+      </c>
+      <c r="W8" s="2">
+        <v>11.859356460000001</v>
+      </c>
+      <c r="X8" s="2">
+        <v>10.642857142857142</v>
+      </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -3778,6 +5193,42 @@
       <c r="L9" s="2">
         <v>13.31891891891892</v>
       </c>
+      <c r="M9">
+        <v>43.8</v>
+      </c>
+      <c r="N9">
+        <v>911</v>
+      </c>
+      <c r="O9" s="1">
+        <v>3.44</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0.86186481663692605</v>
+      </c>
+      <c r="Q9">
+        <v>390.1</v>
+      </c>
+      <c r="R9">
+        <v>299</v>
+      </c>
+      <c r="S9">
+        <v>44.5</v>
+      </c>
+      <c r="T9">
+        <v>860</v>
+      </c>
+      <c r="U9" s="1">
+        <v>5.4866666666666601</v>
+      </c>
+      <c r="V9" s="1">
+        <v>1.3037883725205099</v>
+      </c>
+      <c r="W9" s="2">
+        <v>13.81090605</v>
+      </c>
+      <c r="X9" s="2">
+        <v>13.31891891891892</v>
+      </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -3816,6 +5267,42 @@
       <c r="L10" s="2">
         <v>15.135</v>
       </c>
+      <c r="M10">
+        <v>43.3</v>
+      </c>
+      <c r="N10">
+        <v>1009</v>
+      </c>
+      <c r="O10" s="1">
+        <v>4.62</v>
+      </c>
+      <c r="P10" s="1">
+        <v>1.0901097540209601</v>
+      </c>
+      <c r="Q10">
+        <v>282.7</v>
+      </c>
+      <c r="R10">
+        <v>301</v>
+      </c>
+      <c r="S10">
+        <v>41.3</v>
+      </c>
+      <c r="T10">
+        <v>957</v>
+      </c>
+      <c r="U10" s="1">
+        <v>3.91333333333333</v>
+      </c>
+      <c r="V10" s="1">
+        <v>0.93909346089325096</v>
+      </c>
+      <c r="W10" s="2">
+        <v>12.40419234</v>
+      </c>
+      <c r="X10" s="2">
+        <v>15.135</v>
+      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -3854,6 +5341,42 @@
       <c r="L11" s="2">
         <v>12.588888888888889</v>
       </c>
+      <c r="M11">
+        <v>44.3</v>
+      </c>
+      <c r="N11">
+        <v>999</v>
+      </c>
+      <c r="O11" s="1">
+        <v>4.3333333333333304</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0.93600732295914102</v>
+      </c>
+      <c r="Q11">
+        <v>315</v>
+      </c>
+      <c r="R11">
+        <v>301</v>
+      </c>
+      <c r="S11">
+        <v>40</v>
+      </c>
+      <c r="T11">
+        <v>967</v>
+      </c>
+      <c r="U11" s="1">
+        <v>5.17</v>
+      </c>
+      <c r="V11" s="1">
+        <v>1.0463899546564299</v>
+      </c>
+      <c r="W11" s="2">
+        <v>12.980670249999999</v>
+      </c>
+      <c r="X11" s="2">
+        <v>12.588888888888889</v>
+      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -3892,6 +5415,42 @@
       <c r="L12" s="2">
         <v>12.28</v>
       </c>
+      <c r="M12">
+        <v>39.9</v>
+      </c>
+      <c r="N12">
+        <v>954</v>
+      </c>
+      <c r="O12" s="1">
+        <v>5.0699999999999896</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0.76159054198027298</v>
+      </c>
+      <c r="Q12">
+        <v>258.39999999999998</v>
+      </c>
+      <c r="R12">
+        <v>299</v>
+      </c>
+      <c r="S12">
+        <v>43.8</v>
+      </c>
+      <c r="T12">
+        <v>911</v>
+      </c>
+      <c r="U12" s="1">
+        <v>3.44</v>
+      </c>
+      <c r="V12" s="1">
+        <v>0.86186481663692605</v>
+      </c>
+      <c r="W12" s="2">
+        <v>11.972047160000001</v>
+      </c>
+      <c r="X12" s="2">
+        <v>12.28</v>
+      </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -3930,6 +5489,42 @@
       <c r="L13" s="2">
         <v>12.725</v>
       </c>
+      <c r="M13">
+        <v>39.1</v>
+      </c>
+      <c r="N13">
+        <v>912</v>
+      </c>
+      <c r="O13" s="1">
+        <v>6.0333333333333297</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0.88524590163934402</v>
+      </c>
+      <c r="Q13">
+        <v>352.1</v>
+      </c>
+      <c r="R13">
+        <v>322</v>
+      </c>
+      <c r="S13">
+        <v>43.3</v>
+      </c>
+      <c r="T13">
+        <v>1009</v>
+      </c>
+      <c r="U13" s="1">
+        <v>4.62</v>
+      </c>
+      <c r="V13" s="1">
+        <v>1.0901097540209601</v>
+      </c>
+      <c r="W13" s="2">
+        <v>11.57489485</v>
+      </c>
+      <c r="X13" s="2">
+        <v>12.725</v>
+      </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -3968,6 +5563,42 @@
       <c r="L14" s="2">
         <v>13.112500000000001</v>
       </c>
+      <c r="M14">
+        <v>39.5</v>
+      </c>
+      <c r="N14">
+        <v>947</v>
+      </c>
+      <c r="O14" s="1">
+        <v>5.3466666666666596</v>
+      </c>
+      <c r="P14" s="1">
+        <v>1.28514761119106</v>
+      </c>
+      <c r="Q14">
+        <v>281.2</v>
+      </c>
+      <c r="R14">
+        <v>300</v>
+      </c>
+      <c r="S14">
+        <v>44.3</v>
+      </c>
+      <c r="T14">
+        <v>999</v>
+      </c>
+      <c r="U14" s="1">
+        <v>4.3333333333333304</v>
+      </c>
+      <c r="V14" s="1">
+        <v>0.93600732295914102</v>
+      </c>
+      <c r="W14" s="2">
+        <v>12.529942569999999</v>
+      </c>
+      <c r="X14" s="2">
+        <v>13.112500000000001</v>
+      </c>
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
@@ -4007,6 +5638,42 @@
       <c r="L15" s="2">
         <v>13.309090909090909</v>
       </c>
+      <c r="M15">
+        <v>41.3</v>
+      </c>
+      <c r="N15">
+        <v>965</v>
+      </c>
+      <c r="O15" s="1">
+        <v>4.2033333333333296</v>
+      </c>
+      <c r="P15" s="1">
+        <v>0.99376778214334105</v>
+      </c>
+      <c r="Q15">
+        <v>247.2</v>
+      </c>
+      <c r="R15">
+        <v>339</v>
+      </c>
+      <c r="S15">
+        <v>42.9</v>
+      </c>
+      <c r="T15">
+        <v>1048</v>
+      </c>
+      <c r="U15" s="1">
+        <v>5.7066666666666599</v>
+      </c>
+      <c r="V15" s="1">
+        <v>0.72820467500331398</v>
+      </c>
+      <c r="W15" s="2">
+        <v>12.966400200000001</v>
+      </c>
+      <c r="X15" s="2">
+        <v>13.309090909090909</v>
+      </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="F16">
@@ -4030,8 +5697,44 @@
       <c r="L16" s="2">
         <v>11.176923076923078</v>
       </c>
-    </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="N16">
+        <v>787</v>
+      </c>
+      <c r="O16" s="1">
+        <v>5.5133333333333301</v>
+      </c>
+      <c r="P16" s="1">
+        <v>2.10344565877352</v>
+      </c>
+      <c r="Q16">
+        <v>221.6</v>
+      </c>
+      <c r="R16">
+        <v>290</v>
+      </c>
+      <c r="S16">
+        <v>39.9</v>
+      </c>
+      <c r="T16">
+        <v>954</v>
+      </c>
+      <c r="U16" s="1">
+        <v>5.0699999999999896</v>
+      </c>
+      <c r="V16" s="1">
+        <v>0.76159054198027298</v>
+      </c>
+      <c r="W16" s="2">
+        <v>12.04823423</v>
+      </c>
+      <c r="X16" s="2">
+        <v>11.176923076923078</v>
+      </c>
+    </row>
+    <row r="17" spans="4:24" x14ac:dyDescent="0.25">
       <c r="F17">
         <v>2008</v>
       </c>
@@ -4053,8 +5756,44 @@
       <c r="L17" s="2">
         <v>15.042857142857141</v>
       </c>
-    </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="N17">
+        <v>917</v>
+      </c>
+      <c r="O17" s="1">
+        <v>3.67</v>
+      </c>
+      <c r="P17" s="1">
+        <v>1.3014272157198401</v>
+      </c>
+      <c r="Q17">
+        <v>253.8</v>
+      </c>
+      <c r="R17">
+        <v>286</v>
+      </c>
+      <c r="S17">
+        <v>39.1</v>
+      </c>
+      <c r="T17">
+        <v>912</v>
+      </c>
+      <c r="U17" s="1">
+        <v>6.0333333333333297</v>
+      </c>
+      <c r="V17" s="1">
+        <v>0.88524590163934402</v>
+      </c>
+      <c r="W17" s="2">
+        <v>13.898573499999999</v>
+      </c>
+      <c r="X17" s="2">
+        <v>15.042857142857141</v>
+      </c>
+    </row>
+    <row r="18" spans="4:24" x14ac:dyDescent="0.25">
       <c r="F18">
         <v>2007</v>
       </c>
@@ -4076,8 +5815,44 @@
       <c r="L18" s="2">
         <v>12.1</v>
       </c>
-    </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>40.4</v>
+      </c>
+      <c r="N18">
+        <v>1033</v>
+      </c>
+      <c r="O18" s="1">
+        <v>4.87</v>
+      </c>
+      <c r="P18" s="1">
+        <v>1.4353519372538399</v>
+      </c>
+      <c r="Q18">
+        <v>342.4</v>
+      </c>
+      <c r="R18">
+        <v>301</v>
+      </c>
+      <c r="S18">
+        <v>41.599999999999902</v>
+      </c>
+      <c r="T18">
+        <v>1020</v>
+      </c>
+      <c r="U18" s="1">
+        <v>4.2966666666666598</v>
+      </c>
+      <c r="V18" s="1">
+        <v>1.1362580473883299</v>
+      </c>
+      <c r="W18" s="2">
+        <v>12.848453109999999</v>
+      </c>
+      <c r="X18" s="2">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="19" spans="4:24" x14ac:dyDescent="0.25">
       <c r="F19">
         <v>2006</v>
       </c>
@@ -4099,8 +5874,44 @@
       <c r="L19" s="2">
         <v>12.532142857142857</v>
       </c>
-    </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>42</v>
+      </c>
+      <c r="N19">
+        <v>913</v>
+      </c>
+      <c r="O19" s="1">
+        <v>4.0033333333333303</v>
+      </c>
+      <c r="P19" s="1">
+        <v>1.2647344808174501</v>
+      </c>
+      <c r="Q19">
+        <v>366.1</v>
+      </c>
+      <c r="R19">
+        <v>284</v>
+      </c>
+      <c r="S19">
+        <v>39.5</v>
+      </c>
+      <c r="T19">
+        <v>947</v>
+      </c>
+      <c r="U19" s="1">
+        <v>5.3466666666666596</v>
+      </c>
+      <c r="V19" s="1">
+        <v>1.28514761119106</v>
+      </c>
+      <c r="W19" s="2">
+        <v>13.89854016</v>
+      </c>
+      <c r="X19" s="2">
+        <v>12.532142857142857</v>
+      </c>
+    </row>
+    <row r="20" spans="4:24" x14ac:dyDescent="0.25">
       <c r="F20">
         <v>2005</v>
       </c>
@@ -4122,99 +5933,457 @@
       <c r="L20" s="2">
         <v>14.05</v>
       </c>
-    </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="N20">
+        <v>835</v>
+      </c>
+      <c r="O20" s="1">
+        <v>5.1766666666666596</v>
+      </c>
+      <c r="P20" s="1">
+        <v>1.5003135357878701</v>
+      </c>
+      <c r="Q20">
+        <v>293.39999999999998</v>
+      </c>
+      <c r="R20">
+        <v>295</v>
+      </c>
+      <c r="S20">
+        <v>41.3</v>
+      </c>
+      <c r="T20">
+        <v>965</v>
+      </c>
+      <c r="U20" s="1">
+        <v>4.2033333333333296</v>
+      </c>
+      <c r="V20" s="1">
+        <v>0.99376778214334105</v>
+      </c>
+      <c r="W20" s="2">
+        <v>12.9389074</v>
+      </c>
+      <c r="X20" s="2">
+        <v>14.05</v>
+      </c>
+    </row>
+    <row r="21" spans="4:24" x14ac:dyDescent="0.25">
       <c r="I21">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="J21">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="K21">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="L21" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
+        <v>12.37142857142857</v>
+      </c>
+      <c r="M21">
+        <v>40.4</v>
+      </c>
+      <c r="N21">
+        <v>982</v>
+      </c>
+      <c r="O21" s="1">
+        <v>5.3066666666666604</v>
+      </c>
+      <c r="P21" s="1">
+        <v>0.93681729826432403</v>
+      </c>
+      <c r="Q21">
+        <v>554</v>
+      </c>
+      <c r="R21">
+        <v>263</v>
+      </c>
+      <c r="S21">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="T21">
+        <v>787</v>
+      </c>
+      <c r="U21" s="1">
+        <v>5.5133333333333301</v>
+      </c>
+      <c r="V21" s="1">
+        <v>2.10344565877352</v>
+      </c>
+      <c r="W21" s="2">
+        <v>11.98232353</v>
+      </c>
+      <c r="X21" s="2">
+        <v>12.37142857142857</v>
+      </c>
+    </row>
+    <row r="22" spans="4:24" x14ac:dyDescent="0.25">
       <c r="I22">
-        <v>272</v>
+        <v>494</v>
       </c>
       <c r="J22">
-        <v>290</v>
+        <v>256</v>
       </c>
       <c r="K22">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="L22" s="2">
-        <v>12.37142857142857</v>
-      </c>
-    </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
+        <v>14.416666666666666</v>
+      </c>
+      <c r="M22">
+        <v>42.6</v>
+      </c>
+      <c r="N22">
+        <v>863</v>
+      </c>
+      <c r="O22" s="1">
+        <v>3.7466666666666599</v>
+      </c>
+      <c r="P22" s="1">
+        <v>1.92939708777606</v>
+      </c>
+      <c r="Q22">
+        <v>349.7</v>
+      </c>
+      <c r="R22">
+        <v>268</v>
+      </c>
+      <c r="S22">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="T22">
+        <v>917</v>
+      </c>
+      <c r="U22" s="1">
+        <v>3.67</v>
+      </c>
+      <c r="V22" s="1">
+        <v>1.3014272157198401</v>
+      </c>
+      <c r="W22" s="2">
+        <v>13.413161710000001</v>
+      </c>
+      <c r="X22" s="2">
+        <v>14.416666666666666</v>
+      </c>
+    </row>
+    <row r="23" spans="4:24" x14ac:dyDescent="0.25">
       <c r="I23">
-        <v>494</v>
+        <v>396</v>
       </c>
       <c r="J23">
-        <v>256</v>
+        <v>280</v>
       </c>
       <c r="K23">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="L23" s="2">
-        <v>14.416666666666666</v>
-      </c>
-    </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
+        <v>12.55</v>
+      </c>
+      <c r="M23">
+        <v>41</v>
+      </c>
+      <c r="N23">
+        <v>976</v>
+      </c>
+      <c r="O23" s="1">
+        <v>5.3866666666666596</v>
+      </c>
+      <c r="P23" s="1">
+        <v>1.4126870990734099</v>
+      </c>
+      <c r="Q23">
+        <v>426</v>
+      </c>
+      <c r="R23">
+        <v>297</v>
+      </c>
+      <c r="S23">
+        <v>40.4</v>
+      </c>
+      <c r="T23">
+        <v>1033</v>
+      </c>
+      <c r="U23" s="1">
+        <v>4.87</v>
+      </c>
+      <c r="V23" s="1">
+        <v>1.4353519372538399</v>
+      </c>
+      <c r="W23" s="2">
+        <v>12.67487704</v>
+      </c>
+      <c r="X23" s="2">
+        <v>12.55</v>
+      </c>
+    </row>
+    <row r="24" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D24" s="2"/>
       <c r="I24">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="J24">
-        <v>280</v>
+        <v>245</v>
       </c>
       <c r="K24">
-        <v>1996</v>
+        <v>1993</v>
       </c>
       <c r="L24" s="2">
-        <v>12.55</v>
-      </c>
-    </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
+        <v>12.01</v>
+      </c>
+      <c r="M24">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="N24">
+        <v>837</v>
+      </c>
+      <c r="O24" s="1">
+        <v>4.2033333333333296</v>
+      </c>
+      <c r="P24" s="1">
+        <v>1.63526629149335</v>
+      </c>
+      <c r="Q24">
+        <v>370</v>
+      </c>
+      <c r="R24">
+        <v>293</v>
+      </c>
+      <c r="S24">
+        <v>42</v>
+      </c>
+      <c r="T24">
+        <v>913</v>
+      </c>
+      <c r="U24" s="1">
+        <v>4.0033333333333303</v>
+      </c>
+      <c r="V24" s="1">
+        <v>1.2647344808174501</v>
+      </c>
+      <c r="W24" s="2">
+        <v>12.493339020000001</v>
+      </c>
+      <c r="X24" s="2">
+        <v>12.01</v>
+      </c>
+    </row>
+    <row r="25" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D25" s="2"/>
       <c r="I25">
+        <v>342</v>
+      </c>
+      <c r="J25">
+        <v>267</v>
+      </c>
+      <c r="K25">
+        <v>1992</v>
+      </c>
+      <c r="L25" s="2">
+        <v>12.753846153846153</v>
+      </c>
+      <c r="M25">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="N25">
+        <v>734</v>
+      </c>
+      <c r="O25" s="1">
+        <v>5.6866666666666603</v>
+      </c>
+      <c r="P25" s="1">
+        <v>1.2822816079047801</v>
+      </c>
+      <c r="Q25">
+        <v>418</v>
+      </c>
+      <c r="R25">
+        <v>279</v>
+      </c>
+      <c r="S25">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="T25">
+        <v>835</v>
+      </c>
+      <c r="U25" s="1">
+        <v>5.1766666666666596</v>
+      </c>
+      <c r="V25" s="1">
+        <v>1.5003135357878701</v>
+      </c>
+      <c r="W25" s="2">
+        <v>12.2148875</v>
+      </c>
+      <c r="X25" s="2">
+        <v>12.753846153846153</v>
+      </c>
+    </row>
+    <row r="26" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D26" s="2"/>
+      <c r="Q26">
+        <v>220</v>
+      </c>
+      <c r="R26">
+        <v>302</v>
+      </c>
+      <c r="S26">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="T26">
+        <v>946</v>
+      </c>
+      <c r="U26" s="1">
+        <v>4.1133333333333297</v>
+      </c>
+      <c r="V26" s="1">
+        <v>0.72903769005992702</v>
+      </c>
+    </row>
+    <row r="27" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D27" s="2"/>
+      <c r="Q27">
+        <v>272</v>
+      </c>
+      <c r="R27">
+        <v>290</v>
+      </c>
+      <c r="S27">
+        <v>40.4</v>
+      </c>
+      <c r="T27">
+        <v>982</v>
+      </c>
+      <c r="U27" s="1">
+        <v>5.3066666666666604</v>
+      </c>
+      <c r="V27" s="1">
+        <v>0.93681729826432403</v>
+      </c>
+    </row>
+    <row r="28" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D28" s="2"/>
+      <c r="Q28">
+        <v>494</v>
+      </c>
+      <c r="R28">
+        <v>256</v>
+      </c>
+      <c r="S28">
+        <v>42.6</v>
+      </c>
+      <c r="T28">
+        <v>863</v>
+      </c>
+      <c r="U28" s="1">
+        <v>3.7466666666666599</v>
+      </c>
+      <c r="V28" s="1">
+        <v>1.92939708777606</v>
+      </c>
+    </row>
+    <row r="29" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="Q29">
+        <v>396</v>
+      </c>
+      <c r="R29">
+        <v>280</v>
+      </c>
+      <c r="S29">
+        <v>41</v>
+      </c>
+      <c r="T29">
+        <v>976</v>
+      </c>
+      <c r="U29" s="1">
+        <v>5.3866666666666596</v>
+      </c>
+      <c r="V29" s="1">
+        <v>1.4126870990734099</v>
+      </c>
+    </row>
+    <row r="30" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="Q30">
+        <v>346.3</v>
+      </c>
+      <c r="R30">
+        <v>291</v>
+      </c>
+      <c r="S30">
+        <v>39.699999999999903</v>
+      </c>
+      <c r="T30">
+        <v>918</v>
+      </c>
+      <c r="U30" s="1">
+        <v>2.9866666666666601</v>
+      </c>
+      <c r="V30" s="1">
+        <v>1.19015706086538</v>
+      </c>
+    </row>
+    <row r="31" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="Q31">
+        <v>216.9</v>
+      </c>
+      <c r="R31">
+        <v>279</v>
+      </c>
+      <c r="S31">
+        <v>36.9</v>
+      </c>
+      <c r="T31">
+        <v>804</v>
+      </c>
+      <c r="U31" s="1">
+        <v>4.6266666666666598</v>
+      </c>
+      <c r="V31" s="1">
+        <v>0.77636194430524696</v>
+      </c>
+    </row>
+    <row r="32" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="Q32">
         <v>401</v>
       </c>
-      <c r="J25">
+      <c r="R32">
         <v>245</v>
       </c>
-      <c r="K25">
-        <v>1993</v>
-      </c>
-      <c r="L25" s="2">
-        <v>12.01</v>
-      </c>
-    </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D26" s="2"/>
-      <c r="I26">
+      <c r="S32">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="T32">
+        <v>837</v>
+      </c>
+      <c r="U32" s="1">
+        <v>4.2033333333333296</v>
+      </c>
+      <c r="V32" s="1">
+        <v>1.63526629149335</v>
+      </c>
+    </row>
+    <row r="33" spans="17:22" x14ac:dyDescent="0.25">
+      <c r="Q33">
         <v>342</v>
       </c>
-      <c r="J26">
+      <c r="R33">
         <v>267</v>
       </c>
-      <c r="K26">
-        <v>1992</v>
-      </c>
-      <c r="L26" s="2">
-        <v>12.753846153846153</v>
-      </c>
-    </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D28" s="2"/>
+      <c r="S33">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="T33">
+        <v>734</v>
+      </c>
+      <c r="U33" s="1">
+        <v>5.6866666666666603</v>
+      </c>
+      <c r="V33" s="1">
+        <v>1.2822816079047801</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4224,19 +6393,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C320D8-8C60-47DB-B408-A524D6DB1E3A}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:DK117"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection sqref="A1:D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:115" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -4249,13 +6420,52 @@
       <c r="D1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:115" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>267.8</v>
+      </c>
+      <c r="B2">
+        <v>300</v>
+      </c>
       <c r="C2">
         <v>2023</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>33.4</v>
+      </c>
+      <c r="F2">
+        <v>821</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.88983473547700498</v>
+      </c>
+      <c r="I2" s="2">
+        <v>11.21113487</v>
+      </c>
+    </row>
+    <row r="3" spans="1:115" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>360.8</v>
       </c>
@@ -4268,8 +6478,26 @@
       <c r="D3" s="2">
         <v>9.163636363636364</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>33.099999999999902</v>
+      </c>
+      <c r="F3">
+        <v>992</v>
+      </c>
+      <c r="G3" s="1">
+        <v>6.1666666666666599</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1.26383634580355</v>
+      </c>
+      <c r="I3" s="2">
+        <v>10.479931669999999</v>
+      </c>
+      <c r="J3" s="2">
+        <v>9.163636363636364</v>
+      </c>
+    </row>
+    <row r="4" spans="1:115" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>262</v>
       </c>
@@ -4282,13 +6510,52 @@
       <c r="D4" s="2">
         <v>11.660869565217391</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>46.9</v>
+      </c>
+      <c r="F4">
+        <v>901</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4.6666666666666599</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.86507189671966001</v>
+      </c>
+      <c r="I4" s="2">
+        <v>13.31141117</v>
+      </c>
+      <c r="J4" s="2">
+        <v>11.660869565217391</v>
+      </c>
+    </row>
+    <row r="5" spans="1:115" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>385.8</v>
+      </c>
+      <c r="B5">
+        <v>295</v>
+      </c>
       <c r="C5">
         <v>2020</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>41.3</v>
+      </c>
+      <c r="F5">
+        <v>941</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5.6666666666666599</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1.30808483225117</v>
+      </c>
+      <c r="I5" s="2">
+        <v>12.47833582</v>
+      </c>
+    </row>
+    <row r="6" spans="1:115" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>184</v>
       </c>
@@ -4301,13 +6568,52 @@
       <c r="D6" s="2">
         <v>10.877777777777776</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>42.199999999999903</v>
+      </c>
+      <c r="F6">
+        <v>1022</v>
+      </c>
+      <c r="G6" s="1">
+        <v>5.1999999999999904</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.59789761003428099</v>
+      </c>
+      <c r="I6" s="2">
+        <v>10.476951509999999</v>
+      </c>
+      <c r="J6" s="2">
+        <v>10.877777777777776</v>
+      </c>
+    </row>
+    <row r="7" spans="1:115" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>280.2</v>
+      </c>
+      <c r="B7">
+        <v>315</v>
+      </c>
       <c r="C7">
         <v>2018</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>41.7</v>
+      </c>
+      <c r="F7">
+        <v>931</v>
+      </c>
+      <c r="G7" s="1">
+        <v>6.1999999999999904</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.88934029485979005</v>
+      </c>
+      <c r="I7" s="2">
+        <v>10.436777230000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:115" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>248.9</v>
       </c>
@@ -4320,8 +6626,26 @@
       <c r="D8" s="2">
         <v>11.562068965517241</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>36.9</v>
+      </c>
+      <c r="F8">
+        <v>908</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4.6533333333333298</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.85631224949684304</v>
+      </c>
+      <c r="I8" s="2">
+        <v>12.038451540000001</v>
+      </c>
+      <c r="J8" s="2">
+        <v>11.562068965517241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:115" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>390.1</v>
       </c>
@@ -4334,8 +6658,41 @@
       <c r="D9" s="2">
         <v>13.473333333333333</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>44.5</v>
+      </c>
+      <c r="F9">
+        <v>860</v>
+      </c>
+      <c r="G9" s="1">
+        <v>5.4866666666666601</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1.3037883725205099</v>
+      </c>
+      <c r="I9" s="2">
+        <v>13.5054663</v>
+      </c>
+      <c r="J9" s="2">
+        <v>13.473333333333333</v>
+      </c>
+      <c r="DG9" t="s">
+        <v>37</v>
+      </c>
+      <c r="DH9" t="s">
+        <v>38</v>
+      </c>
+      <c r="DI9" t="s">
+        <v>36</v>
+      </c>
+      <c r="DJ9" t="s">
+        <v>39</v>
+      </c>
+      <c r="DK9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:115" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>282.7</v>
       </c>
@@ -4348,8 +6705,27 @@
       <c r="D10" s="2">
         <v>12.314285714285713</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>41.3</v>
+      </c>
+      <c r="F10">
+        <v>957</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3.91333333333333</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.93909346089325096</v>
+      </c>
+      <c r="I10" s="2">
+        <v>12.84617278</v>
+      </c>
+      <c r="J10" s="2">
+        <v>12.314285714285713</v>
+      </c>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:115" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>315</v>
       </c>
@@ -4362,8 +6738,26 @@
       <c r="D11" s="2">
         <v>10.642857142857142</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>40</v>
+      </c>
+      <c r="F11">
+        <v>967</v>
+      </c>
+      <c r="G11" s="1">
+        <v>5.17</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1.0463899546564299</v>
+      </c>
+      <c r="I11" s="2">
+        <v>11.859356460000001</v>
+      </c>
+      <c r="J11" s="2">
+        <v>10.642857142857142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:115" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>258.39999999999998</v>
       </c>
@@ -4376,8 +6770,26 @@
       <c r="D12" s="2">
         <v>13.31891891891892</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>43.8</v>
+      </c>
+      <c r="F12">
+        <v>911</v>
+      </c>
+      <c r="G12" s="1">
+        <v>3.44</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.86186481663692605</v>
+      </c>
+      <c r="I12" s="2">
+        <v>13.81090605</v>
+      </c>
+      <c r="J12" s="2">
+        <v>13.31891891891892</v>
+      </c>
+    </row>
+    <row r="13" spans="1:115" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>352.1</v>
       </c>
@@ -4390,8 +6802,26 @@
       <c r="D13" s="2">
         <v>15.135</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>43.3</v>
+      </c>
+      <c r="F13">
+        <v>1009</v>
+      </c>
+      <c r="G13" s="1">
+        <v>4.62</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1.0901097540209601</v>
+      </c>
+      <c r="I13" s="2">
+        <v>12.40419234</v>
+      </c>
+      <c r="J13" s="2">
+        <v>15.135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:115" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>281.2</v>
       </c>
@@ -4404,13 +6834,54 @@
       <c r="D14" s="2">
         <v>12.588888888888889</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>44.3</v>
+      </c>
+      <c r="F14">
+        <v>999</v>
+      </c>
+      <c r="G14" s="1">
+        <v>4.3333333333333304</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.93600732295914102</v>
+      </c>
+      <c r="I14" s="2">
+        <v>12.980670249999999</v>
+      </c>
+      <c r="J14" s="2">
+        <v>12.588888888888889</v>
+      </c>
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="1:115" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>247.2</v>
+      </c>
+      <c r="B15">
+        <v>339</v>
+      </c>
       <c r="C15">
         <v>2010</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>42.9</v>
+      </c>
+      <c r="F15">
+        <v>1048</v>
+      </c>
+      <c r="G15" s="1">
+        <v>5.7066666666666599</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.72820467500331398</v>
+      </c>
+      <c r="I15" s="2">
+        <v>8.4879038100000006</v>
+      </c>
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="1:115" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>221.6</v>
       </c>
@@ -4423,8 +6894,27 @@
       <c r="D16" s="2">
         <v>12.28</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>39.9</v>
+      </c>
+      <c r="F16">
+        <v>954</v>
+      </c>
+      <c r="G16" s="1">
+        <v>5.0699999999999896</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.76159054198027298</v>
+      </c>
+      <c r="I16" s="2">
+        <v>11.972047160000001</v>
+      </c>
+      <c r="J16" s="2">
+        <v>12.28</v>
+      </c>
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>253.8</v>
       </c>
@@ -4437,13 +6927,54 @@
       <c r="D17" s="2">
         <v>12.725</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>39.1</v>
+      </c>
+      <c r="F17">
+        <v>912</v>
+      </c>
+      <c r="G17" s="1">
+        <v>6.0333333333333297</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.88524590163934402</v>
+      </c>
+      <c r="I17" s="2">
+        <v>11.57489485</v>
+      </c>
+      <c r="J17" s="2">
+        <v>12.725</v>
+      </c>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>342.4</v>
+      </c>
+      <c r="B18">
+        <v>301</v>
+      </c>
       <c r="C18">
         <v>2007</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>41.599999999999902</v>
+      </c>
+      <c r="F18">
+        <v>1020</v>
+      </c>
+      <c r="G18" s="1">
+        <v>4.2966666666666598</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1.1362580473883299</v>
+      </c>
+      <c r="I18" s="2">
+        <v>12.908599499999999</v>
+      </c>
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>366.1</v>
       </c>
@@ -4456,8 +6987,27 @@
       <c r="D19" s="2">
         <v>13.112500000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>39.5</v>
+      </c>
+      <c r="F19">
+        <v>947</v>
+      </c>
+      <c r="G19" s="1">
+        <v>5.3466666666666596</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1.28514761119106</v>
+      </c>
+      <c r="I19" s="2">
+        <v>12.529942569999999</v>
+      </c>
+      <c r="J19" s="2">
+        <v>13.112500000000001</v>
+      </c>
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>293.39999999999998</v>
       </c>
@@ -4470,8 +7020,27 @@
       <c r="D20" s="2">
         <v>13.309090909090909</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>41.3</v>
+      </c>
+      <c r="F20">
+        <v>965</v>
+      </c>
+      <c r="G20" s="1">
+        <v>4.2033333333333296</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.99376778214334105</v>
+      </c>
+      <c r="I20" s="2">
+        <v>12.966400200000001</v>
+      </c>
+      <c r="J20" s="2">
+        <v>13.309090909090909</v>
+      </c>
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>554</v>
       </c>
@@ -4484,8 +7053,27 @@
       <c r="D21" s="2">
         <v>11.176923076923078</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="F21">
+        <v>787</v>
+      </c>
+      <c r="G21" s="1">
+        <v>5.5133333333333301</v>
+      </c>
+      <c r="H21" s="1">
+        <v>2.10344565877352</v>
+      </c>
+      <c r="I21" s="2">
+        <v>12.04823423</v>
+      </c>
+      <c r="J21" s="2">
+        <v>11.176923076923078</v>
+      </c>
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>349.7</v>
       </c>
@@ -4498,8 +7086,27 @@
       <c r="D22" s="2">
         <v>15.042857142857141</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="F22">
+        <v>917</v>
+      </c>
+      <c r="G22" s="1">
+        <v>3.67</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1.3014272157198401</v>
+      </c>
+      <c r="I22" s="2">
+        <v>13.898573499999999</v>
+      </c>
+      <c r="J22" s="2">
+        <v>15.042857142857141</v>
+      </c>
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>426</v>
       </c>
@@ -4512,8 +7119,27 @@
       <c r="D23" s="2">
         <v>12.1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>40.4</v>
+      </c>
+      <c r="F23">
+        <v>1033</v>
+      </c>
+      <c r="G23" s="1">
+        <v>4.87</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1.4353519372538399</v>
+      </c>
+      <c r="I23" s="2">
+        <v>12.848453109999999</v>
+      </c>
+      <c r="J23" s="2">
+        <v>12.1</v>
+      </c>
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>370</v>
       </c>
@@ -4526,8 +7152,27 @@
       <c r="D24" s="2">
         <v>12.532142857142857</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>42</v>
+      </c>
+      <c r="F24">
+        <v>913</v>
+      </c>
+      <c r="G24" s="1">
+        <v>4.0033333333333303</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1.2647344808174501</v>
+      </c>
+      <c r="I24" s="2">
+        <v>13.89854016</v>
+      </c>
+      <c r="J24" s="2">
+        <v>12.532142857142857</v>
+      </c>
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>418</v>
       </c>
@@ -4540,8 +7185,27 @@
       <c r="D25" s="2">
         <v>14.05</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="F25">
+        <v>835</v>
+      </c>
+      <c r="G25" s="1">
+        <v>5.1766666666666596</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1.5003135357878701</v>
+      </c>
+      <c r="I25" s="2">
+        <v>12.9389074</v>
+      </c>
+      <c r="J25" s="2">
+        <v>14.05</v>
+      </c>
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>220</v>
       </c>
@@ -4554,8 +7218,25 @@
       <c r="D26" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="F26">
+        <v>946</v>
+      </c>
+      <c r="G26" s="1">
+        <v>4.1133333333333297</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.72903769005992702</v>
+      </c>
+      <c r="I26" s="2">
+        <v>11.83763589</v>
+      </c>
+      <c r="J26" s="2"/>
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>272</v>
       </c>
@@ -4568,8 +7249,27 @@
       <c r="D27" s="2">
         <v>12.37142857142857</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>40.4</v>
+      </c>
+      <c r="F27">
+        <v>982</v>
+      </c>
+      <c r="G27" s="1">
+        <v>5.3066666666666604</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.93681729826432403</v>
+      </c>
+      <c r="I27" s="2">
+        <v>11.98232353</v>
+      </c>
+      <c r="J27" s="2">
+        <v>12.37142857142857</v>
+      </c>
+      <c r="N27" s="1"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>494</v>
       </c>
@@ -4582,8 +7282,27 @@
       <c r="D28" s="2">
         <v>14.416666666666666</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>42.6</v>
+      </c>
+      <c r="F28">
+        <v>863</v>
+      </c>
+      <c r="G28" s="1">
+        <v>3.7466666666666599</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1.92939708777606</v>
+      </c>
+      <c r="I28" s="2">
+        <v>13.413161710000001</v>
+      </c>
+      <c r="J28" s="2">
+        <v>14.416666666666666</v>
+      </c>
+      <c r="N28" s="1"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>396</v>
       </c>
@@ -4596,24 +7315,89 @@
       <c r="D29" s="2">
         <v>12.55</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>41</v>
+      </c>
+      <c r="F29">
+        <v>976</v>
+      </c>
+      <c r="G29" s="1">
+        <v>5.3866666666666596</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1.4126870990734099</v>
+      </c>
+      <c r="I29" s="2">
+        <v>12.67487704</v>
+      </c>
+      <c r="J29" s="2">
+        <v>12.55</v>
+      </c>
+      <c r="N29" s="1"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>346.3</v>
+      </c>
+      <c r="B30">
+        <v>291</v>
+      </c>
       <c r="C30">
         <v>1995</v>
       </c>
       <c r="D30" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>39.699999999999903</v>
+      </c>
+      <c r="F30">
+        <v>918</v>
+      </c>
+      <c r="G30" s="1">
+        <v>2.9866666666666601</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1.19015706086538</v>
+      </c>
+      <c r="I30" s="2">
+        <v>14.218488450000001</v>
+      </c>
+      <c r="J30" s="2"/>
+      <c r="N30" s="1"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>216.9</v>
+      </c>
+      <c r="B31">
+        <v>279</v>
+      </c>
       <c r="C31">
         <v>1994</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>36.9</v>
+      </c>
+      <c r="F31">
+        <v>804</v>
+      </c>
+      <c r="G31" s="1">
+        <v>4.6266666666666598</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0.77636194430524696</v>
+      </c>
+      <c r="I31" s="2">
+        <v>12.937180870000001</v>
+      </c>
+      <c r="J31" s="2"/>
+      <c r="N31" s="1"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>401</v>
       </c>
@@ -4626,8 +7410,27 @@
       <c r="D32" s="2">
         <v>12.01</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="F32">
+        <v>837</v>
+      </c>
+      <c r="G32" s="1">
+        <v>4.2033333333333296</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1.63526629149335</v>
+      </c>
+      <c r="I32" s="2">
+        <v>12.493339020000001</v>
+      </c>
+      <c r="J32" s="2">
+        <v>12.01</v>
+      </c>
+      <c r="N32" s="1"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>342</v>
       </c>
@@ -4640,9 +7443,721 @@
       <c r="D33" s="2">
         <v>12.753846153846153</v>
       </c>
+      <c r="E33">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="F33">
+        <v>734</v>
+      </c>
+      <c r="G33" s="1">
+        <v>5.6866666666666603</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1.2822816079047801</v>
+      </c>
+      <c r="I33" s="2">
+        <v>12.2148875</v>
+      </c>
+      <c r="J33" s="2">
+        <v>12.753846153846153</v>
+      </c>
+      <c r="N33" s="1"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>44</v>
+      </c>
+      <c r="F34">
+        <v>925</v>
+      </c>
+      <c r="G34" s="1">
+        <v>3.24</v>
+      </c>
+      <c r="N34" s="1"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="F35">
+        <v>801</v>
+      </c>
+      <c r="G35" s="1">
+        <v>4.9933333333333296</v>
+      </c>
+      <c r="N35" s="1"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="F36">
+        <v>772</v>
+      </c>
+      <c r="G36" s="1">
+        <v>3.35</v>
+      </c>
+      <c r="N36" s="1"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>45.099999999999902</v>
+      </c>
+      <c r="F37">
+        <v>813</v>
+      </c>
+      <c r="G37" s="1">
+        <v>5.43333333333333</v>
+      </c>
+      <c r="N37" s="1"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>39.9</v>
+      </c>
+      <c r="F38">
+        <v>841</v>
+      </c>
+      <c r="G38" s="1">
+        <v>3.06</v>
+      </c>
+      <c r="N38" s="1"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="F39">
+        <v>619</v>
+      </c>
+      <c r="G39" s="1">
+        <v>5.4033333333333298</v>
+      </c>
+      <c r="N39" s="1"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="F40">
+        <v>867</v>
+      </c>
+      <c r="G40" s="1">
+        <v>3.3699999999999899</v>
+      </c>
+      <c r="N40" s="1"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>38.5</v>
+      </c>
+      <c r="F41">
+        <v>962</v>
+      </c>
+      <c r="G41" s="1">
+        <v>5.9899999999999904</v>
+      </c>
+      <c r="N41" s="1"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>41.6</v>
+      </c>
+      <c r="F42">
+        <v>783</v>
+      </c>
+      <c r="G42" s="1">
+        <v>2.5033333333333299</v>
+      </c>
+      <c r="N42" s="1"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="F43">
+        <v>500</v>
+      </c>
+      <c r="G43" s="1">
+        <v>5.2033333333333296</v>
+      </c>
+      <c r="N43" s="1"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>39</v>
+      </c>
+      <c r="F44">
+        <v>622</v>
+      </c>
+      <c r="G44" s="1">
+        <v>2.2899999999999898</v>
+      </c>
+      <c r="N44" s="1"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>38</v>
+      </c>
+      <c r="F45">
+        <v>746</v>
+      </c>
+      <c r="G45" s="1">
+        <v>4.67</v>
+      </c>
+      <c r="N45" s="1"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>35.1</v>
+      </c>
+      <c r="F46">
+        <v>931</v>
+      </c>
+      <c r="G46" s="1">
+        <v>3.5033333333333299</v>
+      </c>
+      <c r="N46" s="1"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>35.4</v>
+      </c>
+      <c r="F47">
+        <v>840</v>
+      </c>
+      <c r="G47" s="1">
+        <v>5.8566666666666602</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>42.099999999999902</v>
+      </c>
+      <c r="F48">
+        <v>790</v>
+      </c>
+      <c r="G48" s="1">
+        <v>3.03666666666666</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="F49">
+        <v>779</v>
+      </c>
+      <c r="G49" s="1">
+        <v>5.3066666666666604</v>
+      </c>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>38.4</v>
+      </c>
+      <c r="F50">
+        <v>967</v>
+      </c>
+      <c r="G50" s="1">
+        <v>2.1066666666666598</v>
+      </c>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="F51">
+        <v>858</v>
+      </c>
+      <c r="G51" s="1">
+        <v>4.5233333333333299</v>
+      </c>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>38.9</v>
+      </c>
+      <c r="F52">
+        <v>792</v>
+      </c>
+      <c r="G52" s="1">
+        <v>2.82666666666666</v>
+      </c>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>41.6</v>
+      </c>
+      <c r="F53">
+        <v>982</v>
+      </c>
+      <c r="G53" s="1">
+        <v>5.18</v>
+      </c>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="F54">
+        <v>990</v>
+      </c>
+      <c r="G54" s="1">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="F55">
+        <v>976</v>
+      </c>
+      <c r="G55" s="1">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="F56">
+        <v>865</v>
+      </c>
+      <c r="G56" s="1">
+        <v>2.46</v>
+      </c>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>34.9</v>
+      </c>
+      <c r="F57">
+        <v>898</v>
+      </c>
+      <c r="G57" s="1">
+        <v>5.5466666666666598</v>
+      </c>
+    </row>
+    <row r="58" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="F58">
+        <v>911</v>
+      </c>
+      <c r="G58" s="1">
+        <v>2.8166666666666602</v>
+      </c>
+    </row>
+    <row r="59" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="F59">
+        <v>925</v>
+      </c>
+      <c r="G59" s="1">
+        <v>5.93</v>
+      </c>
+    </row>
+    <row r="60" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="F60">
+        <v>966</v>
+      </c>
+      <c r="G60" s="1">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="61" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>39</v>
+      </c>
+      <c r="F61">
+        <v>908</v>
+      </c>
+      <c r="G61" s="1">
+        <v>6.32666666666666</v>
+      </c>
+    </row>
+    <row r="62" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="F62">
+        <v>1096</v>
+      </c>
+      <c r="G62" s="1">
+        <v>2.5933333333333302</v>
+      </c>
+    </row>
+    <row r="63" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>34.6</v>
+      </c>
+      <c r="F63">
+        <v>935</v>
+      </c>
+      <c r="G63" s="1">
+        <v>6.1766666666666596</v>
+      </c>
+    </row>
+    <row r="64" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>38</v>
+      </c>
+      <c r="F64">
+        <v>850</v>
+      </c>
+      <c r="G64" s="1">
+        <v>1.93</v>
+      </c>
+    </row>
+    <row r="65" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="G65" s="1">
+        <v>5.6566666666666601</v>
+      </c>
+    </row>
+    <row r="66" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="G66" s="1">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="G67" s="1">
+        <v>6.64333333333333</v>
+      </c>
+    </row>
+    <row r="68" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="G68" s="1">
+        <v>3.30666666666666</v>
+      </c>
+    </row>
+    <row r="69" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>35.9</v>
+      </c>
+      <c r="G69" s="1">
+        <v>5.9266666666666596</v>
+      </c>
+    </row>
+    <row r="70" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>37</v>
+      </c>
+      <c r="G70" s="1">
+        <v>1.8333333333333299</v>
+      </c>
+    </row>
+    <row r="71" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <v>41.9</v>
+      </c>
+      <c r="G71" s="1">
+        <v>5.72</v>
+      </c>
+    </row>
+    <row r="72" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>39.9</v>
+      </c>
+      <c r="G72" s="1">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="73" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="G73" s="1">
+        <v>6.41</v>
+      </c>
+    </row>
+    <row r="74" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="G74" s="1">
+        <v>2.6799999999999899</v>
+      </c>
+    </row>
+    <row r="75" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="G75" s="1">
+        <v>6.7166666666666597</v>
+      </c>
+    </row>
+    <row r="76" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>37</v>
+      </c>
+      <c r="G76" s="1">
+        <v>2.09666666666666</v>
+      </c>
+    </row>
+    <row r="77" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>42</v>
+      </c>
+      <c r="G77" s="1">
+        <v>5.6566666666666601</v>
+      </c>
+    </row>
+    <row r="78" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="G78" s="1">
+        <v>1.9266666666666601</v>
+      </c>
+    </row>
+    <row r="79" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <v>34.1</v>
+      </c>
+      <c r="G79" s="1">
+        <v>6.5533333333333301</v>
+      </c>
+    </row>
+    <row r="80" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="G80" s="1">
+        <v>2.07666666666666</v>
+      </c>
+    </row>
+    <row r="81" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="G81" s="1">
+        <v>5.6966666666666601</v>
+      </c>
+    </row>
+    <row r="82" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="G82" s="1">
+        <v>2.12333333333333</v>
+      </c>
+    </row>
+    <row r="83" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="G83" s="1">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="84" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>39.5</v>
+      </c>
+      <c r="G84" s="1">
+        <v>2.2166666666666601</v>
+      </c>
+    </row>
+    <row r="85" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="G85" s="1">
+        <v>6.53666666666666</v>
+      </c>
+    </row>
+    <row r="86" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>38.5</v>
+      </c>
+      <c r="G86" s="1">
+        <v>2.0233333333333299</v>
+      </c>
+    </row>
+    <row r="87" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="G87" s="1">
+        <v>6.2066666666666599</v>
+      </c>
+    </row>
+    <row r="88" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G88" s="1">
+        <v>2.8233333333333301</v>
+      </c>
+    </row>
+    <row r="89" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G89" s="1">
+        <v>7.1133333333333297</v>
+      </c>
+    </row>
+    <row r="90" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G90" s="1">
+        <v>2.0933333333333302</v>
+      </c>
+    </row>
+    <row r="91" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G91" s="1">
+        <v>5.3133333333333299</v>
+      </c>
+    </row>
+    <row r="92" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G92" s="1">
+        <v>3.5666666666666602</v>
+      </c>
+    </row>
+    <row r="93" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G93" s="1">
+        <v>5.98</v>
+      </c>
+    </row>
+    <row r="94" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G94" s="1">
+        <v>3.03</v>
+      </c>
+    </row>
+    <row r="95" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G95" s="1">
+        <v>6.2766666666666602</v>
+      </c>
+    </row>
+    <row r="96" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G96" s="1">
+        <v>3.3699999999999899</v>
+      </c>
+    </row>
+    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G97" s="1">
+        <v>5.9933333333333296</v>
+      </c>
+    </row>
+    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G98" s="1">
+        <v>2.2466666666666599</v>
+      </c>
+    </row>
+    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G99" s="1">
+        <v>5.2033333333333296</v>
+      </c>
+    </row>
+    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G100" s="1">
+        <v>4.2333333333333298</v>
+      </c>
+    </row>
+    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G101" s="1">
+        <v>7.0866666666666598</v>
+      </c>
+    </row>
+    <row r="102" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G102" s="1">
+        <v>4.7399999999999904</v>
+      </c>
+    </row>
+    <row r="103" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G103" s="1">
+        <v>6.14333333333333</v>
+      </c>
+    </row>
+    <row r="104" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G104" s="1">
+        <v>3.09666666666666</v>
+      </c>
+    </row>
+    <row r="105" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G105" s="1">
+        <v>5.5233333333333299</v>
+      </c>
+    </row>
+    <row r="106" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G106" s="1">
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="107" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G107" s="1">
+        <v>5.00999999999999</v>
+      </c>
+    </row>
+    <row r="108" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G108" s="1">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="109" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G109" s="1">
+        <v>6.2966666666666598</v>
+      </c>
+    </row>
+    <row r="110" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G110" s="1">
+        <v>3.53666666666666</v>
+      </c>
+    </row>
+    <row r="111" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G111" s="1">
+        <v>6.44</v>
+      </c>
+    </row>
+    <row r="112" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G112" s="1">
+        <v>2.62333333333333</v>
+      </c>
+    </row>
+    <row r="113" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G113" s="1">
+        <v>5.0066666666666597</v>
+      </c>
+    </row>
+    <row r="114" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G114" s="1">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="115" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G115" s="1">
+        <v>6.4233333333333302</v>
+      </c>
+    </row>
+    <row r="116" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G116" s="1">
+        <v>3.9233333333333298</v>
+      </c>
+    </row>
+    <row r="117" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G117" s="1">
+        <v>5.9066666666666601</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N14:O45">
+    <sortCondition descending="1" ref="O14:O45"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
feat: xls data update
</commit_message>
<xml_diff>
--- a/protein_Belgorod.xlsx
+++ b/protein_Belgorod.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkd\dev\diploma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189E4F2E-50C7-4E43-BC87-8D4BF3AB808F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1C5174-5841-437C-AEDB-063A3CE0B4E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4ADC32DF-F1DC-4277-9E07-398DF3F93614}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>year</t>
   </si>
@@ -164,9 +164,6 @@
     <t>HTC_v</t>
   </si>
   <si>
-    <t>R_v_full</t>
-  </si>
-  <si>
     <t>T_v_full</t>
   </si>
   <si>
@@ -184,6 +181,9 @@
   <si>
     <t>protein_forecast</t>
   </si>
+  <si>
+    <t>R_v_full</t>
+  </si>
 </sst>
 </file>
 
@@ -192,17 +192,8 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -231,11 +222,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1402,6 +1392,111 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>full!$C$2:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>full!$I$2:$I$33</c:f>
@@ -1540,6 +1635,111 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>full!$C$2:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>full!$J$2:$J$33</c:f>
@@ -1576,6 +1776,9 @@
                 <c:pt idx="12">
                   <c:v>12.588888888888889</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.95</c:v>
+                </c:pt>
                 <c:pt idx="14">
                   <c:v>12.28</c:v>
                 </c:pt>
@@ -1602,6 +1805,9 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>14.05</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11.8</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>12.37142857142857</c:v>
@@ -4126,16 +4332,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>295274</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>247649</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4542,10 +4748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{139D87CC-99BC-47AF-8614-82F5A31FEE7F}">
-  <dimension ref="A1:Z33"/>
+  <dimension ref="A1:AC33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4558,13 +4764,14 @@
     <col min="9" max="10" width="19" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4589,56 +4796,53 @@
       <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>30</v>
-      </c>
       <c r="K1" t="s">
         <v>32</v>
       </c>
       <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" t="s">
         <v>33</v>
       </c>
-      <c r="M1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" t="s">
-        <v>42</v>
-      </c>
       <c r="Q1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="R1" t="s">
-        <v>44</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" t="s">
-        <v>47</v>
-      </c>
-      <c r="V1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="W1" t="s">
         <v>49</v>
       </c>
       <c r="X1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2022</v>
       </c>
@@ -4663,56 +4867,53 @@
       <c r="H2">
         <v>64</v>
       </c>
-      <c r="I2">
-        <v>360.8</v>
-      </c>
-      <c r="J2">
-        <v>285</v>
-      </c>
       <c r="K2">
         <v>2022</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2">
+        <v>33.099999999999902</v>
+      </c>
+      <c r="M2">
+        <v>992</v>
+      </c>
+      <c r="N2" s="1">
+        <v>6.1666666666666599</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1.26383634580355</v>
+      </c>
+      <c r="P2" s="2">
         <v>9.163636363636364</v>
       </c>
-      <c r="M2">
-        <v>33.099999999999902</v>
-      </c>
-      <c r="N2">
-        <v>992</v>
-      </c>
-      <c r="O2" s="1">
-        <v>6.1666666666666599</v>
-      </c>
-      <c r="P2" s="1">
-        <v>1.26383634580355</v>
-      </c>
       <c r="Q2">
+        <v>360.8</v>
+      </c>
+      <c r="R2">
+        <v>285</v>
+      </c>
+      <c r="W2">
         <v>267.8</v>
       </c>
-      <c r="R2">
+      <c r="X2">
         <v>300</v>
       </c>
-      <c r="S2">
+      <c r="Y2">
         <v>33.4</v>
       </c>
-      <c r="T2">
+      <c r="Z2">
         <v>821</v>
       </c>
-      <c r="U2" s="1">
+      <c r="AA2" s="1">
         <v>4.8</v>
       </c>
-      <c r="V2" s="1">
+      <c r="AB2" s="1">
         <v>0.88983473547700498</v>
       </c>
-      <c r="W2" s="2">
+      <c r="AC2" s="2">
         <v>10.479931669999999</v>
       </c>
-      <c r="X2" s="2">
-        <v>9.163636363636364</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -4737,56 +4938,53 @@
       <c r="H3">
         <v>66</v>
       </c>
-      <c r="I3">
-        <v>262</v>
-      </c>
-      <c r="J3">
-        <v>302</v>
-      </c>
       <c r="K3">
         <v>2021</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3">
+        <v>46.9</v>
+      </c>
+      <c r="M3">
+        <v>901</v>
+      </c>
+      <c r="N3" s="1">
+        <v>4.6666666666666599</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.86507189671966001</v>
+      </c>
+      <c r="P3" s="2">
         <v>11.660869565217391</v>
       </c>
-      <c r="M3">
-        <v>46.9</v>
-      </c>
-      <c r="N3">
-        <v>901</v>
-      </c>
-      <c r="O3" s="1">
-        <v>4.6666666666666599</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0.86507189671966001</v>
-      </c>
       <c r="Q3">
+        <v>262</v>
+      </c>
+      <c r="R3">
+        <v>302</v>
+      </c>
+      <c r="W3">
         <v>360.8</v>
       </c>
-      <c r="R3">
+      <c r="X3">
         <v>285</v>
       </c>
-      <c r="S3">
+      <c r="Y3">
         <v>33.099999999999902</v>
       </c>
-      <c r="T3">
+      <c r="Z3">
         <v>992</v>
       </c>
-      <c r="U3" s="1">
+      <c r="AA3" s="1">
         <v>6.1666666666666599</v>
       </c>
-      <c r="V3" s="1">
+      <c r="AB3" s="1">
         <v>1.26383634580355</v>
       </c>
-      <c r="W3" s="2">
+      <c r="AC3" s="2">
         <v>13.31141117</v>
       </c>
-      <c r="X3" s="2">
-        <v>11.660869565217391</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2019</v>
       </c>
@@ -4811,56 +5009,53 @@
       <c r="H4">
         <v>61</v>
       </c>
-      <c r="I4">
-        <v>184</v>
-      </c>
-      <c r="J4">
-        <v>307</v>
-      </c>
       <c r="K4">
         <v>2019</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4">
+        <v>42.199999999999903</v>
+      </c>
+      <c r="M4">
+        <v>1022</v>
+      </c>
+      <c r="N4" s="1">
+        <v>5.1999999999999904</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0.59789761003428099</v>
+      </c>
+      <c r="P4" s="2">
         <v>10.877777777777776</v>
       </c>
-      <c r="M4">
-        <v>42.199999999999903</v>
-      </c>
-      <c r="N4">
-        <v>1022</v>
-      </c>
-      <c r="O4" s="1">
-        <v>5.1999999999999904</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0.59789761003428099</v>
-      </c>
       <c r="Q4">
+        <v>184</v>
+      </c>
+      <c r="R4">
+        <v>307</v>
+      </c>
+      <c r="W4">
         <v>262</v>
       </c>
-      <c r="R4">
+      <c r="X4">
         <v>302</v>
       </c>
-      <c r="S4">
+      <c r="Y4">
         <v>46.9</v>
       </c>
-      <c r="T4">
+      <c r="Z4">
         <v>901</v>
       </c>
-      <c r="U4" s="1">
+      <c r="AA4" s="1">
         <v>4.6666666666666599</v>
       </c>
-      <c r="V4" s="1">
+      <c r="AB4" s="1">
         <v>0.86507189671966001</v>
       </c>
-      <c r="W4" s="2">
+      <c r="AC4" s="2">
         <v>10.476951509999999</v>
       </c>
-      <c r="X4" s="2">
-        <v>10.877777777777776</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2017</v>
       </c>
@@ -4885,56 +5080,53 @@
       <c r="H5">
         <v>54</v>
       </c>
-      <c r="I5">
-        <v>248.9</v>
-      </c>
-      <c r="J5">
-        <v>290</v>
-      </c>
       <c r="K5">
         <v>2017</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5">
+        <v>36.9</v>
+      </c>
+      <c r="M5">
+        <v>908</v>
+      </c>
+      <c r="N5" s="1">
+        <v>4.6533333333333298</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0.85631224949684304</v>
+      </c>
+      <c r="P5" s="2">
         <v>11.562068965517241</v>
       </c>
-      <c r="M5">
-        <v>36.9</v>
-      </c>
-      <c r="N5">
-        <v>908</v>
-      </c>
-      <c r="O5" s="1">
-        <v>4.6533333333333298</v>
-      </c>
-      <c r="P5" s="1">
-        <v>0.85631224949684304</v>
-      </c>
       <c r="Q5">
+        <v>248.9</v>
+      </c>
+      <c r="R5">
+        <v>290</v>
+      </c>
+      <c r="W5">
         <v>385.8</v>
       </c>
-      <c r="R5">
+      <c r="X5">
         <v>295</v>
       </c>
-      <c r="S5">
+      <c r="Y5">
         <v>41.3</v>
       </c>
-      <c r="T5">
+      <c r="Z5">
         <v>941</v>
       </c>
-      <c r="U5" s="1">
+      <c r="AA5" s="1">
         <v>5.6666666666666599</v>
       </c>
-      <c r="V5" s="1">
+      <c r="AB5" s="1">
         <v>1.30808483225117</v>
       </c>
-      <c r="W5" s="2">
+      <c r="AC5" s="2">
         <v>12.038451540000001</v>
       </c>
-      <c r="X5" s="2">
-        <v>11.562068965517241</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2016</v>
       </c>
@@ -4959,56 +5151,53 @@
       <c r="H6">
         <v>60</v>
       </c>
-      <c r="I6">
-        <v>390.1</v>
-      </c>
-      <c r="J6">
-        <v>299</v>
-      </c>
       <c r="K6">
         <v>2016</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6">
+        <v>44.5</v>
+      </c>
+      <c r="M6">
+        <v>860</v>
+      </c>
+      <c r="N6" s="1">
+        <v>5.4866666666666601</v>
+      </c>
+      <c r="O6" s="1">
+        <v>1.3037883725205099</v>
+      </c>
+      <c r="P6" s="2">
         <v>13.473333333333333</v>
       </c>
-      <c r="M6">
-        <v>44.5</v>
-      </c>
-      <c r="N6">
-        <v>860</v>
-      </c>
-      <c r="O6" s="1">
-        <v>5.4866666666666601</v>
-      </c>
-      <c r="P6" s="1">
-        <v>1.3037883725205099</v>
-      </c>
       <c r="Q6">
+        <v>390.1</v>
+      </c>
+      <c r="R6">
+        <v>299</v>
+      </c>
+      <c r="W6">
         <v>184</v>
       </c>
-      <c r="R6">
+      <c r="X6">
         <v>307</v>
       </c>
-      <c r="S6">
+      <c r="Y6">
         <v>42.199999999999903</v>
       </c>
-      <c r="T6">
+      <c r="Z6">
         <v>1022</v>
       </c>
-      <c r="U6" s="1">
+      <c r="AA6" s="1">
         <v>5.1999999999999904</v>
       </c>
-      <c r="V6" s="1">
+      <c r="AB6" s="1">
         <v>0.59789761003428099</v>
       </c>
-      <c r="W6" s="2">
+      <c r="AC6" s="2">
         <v>13.5054663</v>
       </c>
-      <c r="X6" s="2">
-        <v>13.473333333333333</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -5033,56 +5222,53 @@
       <c r="H7">
         <v>58</v>
       </c>
-      <c r="I7">
-        <v>282.7</v>
-      </c>
-      <c r="J7">
-        <v>301</v>
-      </c>
       <c r="K7">
         <v>2015</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7">
+        <v>41.3</v>
+      </c>
+      <c r="M7">
+        <v>957</v>
+      </c>
+      <c r="N7" s="1">
+        <v>3.91333333333333</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0.93909346089325096</v>
+      </c>
+      <c r="P7" s="2">
         <v>12.314285714285713</v>
       </c>
-      <c r="M7">
-        <v>41.3</v>
-      </c>
-      <c r="N7">
-        <v>957</v>
-      </c>
-      <c r="O7" s="1">
-        <v>3.91333333333333</v>
-      </c>
-      <c r="P7" s="1">
-        <v>0.93909346089325096</v>
-      </c>
       <c r="Q7">
+        <v>282.7</v>
+      </c>
+      <c r="R7">
+        <v>301</v>
+      </c>
+      <c r="W7">
         <v>280.2</v>
       </c>
-      <c r="R7">
+      <c r="X7">
         <v>315</v>
       </c>
-      <c r="S7">
+      <c r="Y7">
         <v>41.7</v>
       </c>
-      <c r="T7">
+      <c r="Z7">
         <v>931</v>
       </c>
-      <c r="U7" s="1">
+      <c r="AA7" s="1">
         <v>6.1999999999999904</v>
       </c>
-      <c r="V7" s="1">
+      <c r="AB7" s="1">
         <v>0.88934029485979005</v>
       </c>
-      <c r="W7" s="2">
+      <c r="AC7" s="2">
         <v>12.84617278</v>
       </c>
-      <c r="X7" s="2">
-        <v>12.314285714285713</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2014</v>
       </c>
@@ -5107,56 +5293,53 @@
       <c r="H8">
         <v>60</v>
       </c>
-      <c r="I8">
-        <v>315</v>
-      </c>
-      <c r="J8">
-        <v>301</v>
-      </c>
       <c r="K8">
         <v>2014</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8">
+        <v>40</v>
+      </c>
+      <c r="M8">
+        <v>967</v>
+      </c>
+      <c r="N8" s="1">
+        <v>5.17</v>
+      </c>
+      <c r="O8" s="1">
+        <v>1.0463899546564299</v>
+      </c>
+      <c r="P8" s="2">
         <v>10.642857142857142</v>
       </c>
-      <c r="M8">
-        <v>40</v>
-      </c>
-      <c r="N8">
-        <v>967</v>
-      </c>
-      <c r="O8" s="1">
-        <v>5.17</v>
-      </c>
-      <c r="P8" s="1">
-        <v>1.0463899546564299</v>
-      </c>
       <c r="Q8">
+        <v>315</v>
+      </c>
+      <c r="R8">
+        <v>301</v>
+      </c>
+      <c r="W8">
         <v>248.9</v>
       </c>
-      <c r="R8">
+      <c r="X8">
         <v>290</v>
       </c>
-      <c r="S8">
+      <c r="Y8">
         <v>36.9</v>
       </c>
-      <c r="T8">
+      <c r="Z8">
         <v>908</v>
       </c>
-      <c r="U8" s="1">
+      <c r="AA8" s="1">
         <v>4.6533333333333298</v>
       </c>
-      <c r="V8" s="1">
+      <c r="AB8" s="1">
         <v>0.85631224949684304</v>
       </c>
-      <c r="W8" s="2">
+      <c r="AC8" s="2">
         <v>11.859356460000001</v>
       </c>
-      <c r="X8" s="2">
-        <v>10.642857142857142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2013</v>
       </c>
@@ -5181,56 +5364,53 @@
       <c r="H9">
         <v>72</v>
       </c>
-      <c r="I9">
-        <v>258.39999999999998</v>
-      </c>
-      <c r="J9">
-        <v>299</v>
-      </c>
       <c r="K9">
         <v>2013</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9">
+        <v>43.8</v>
+      </c>
+      <c r="M9">
+        <v>911</v>
+      </c>
+      <c r="N9" s="1">
+        <v>3.44</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0.86186481663692605</v>
+      </c>
+      <c r="P9" s="2">
         <v>13.31891891891892</v>
       </c>
-      <c r="M9">
-        <v>43.8</v>
-      </c>
-      <c r="N9">
-        <v>911</v>
-      </c>
-      <c r="O9" s="1">
-        <v>3.44</v>
-      </c>
-      <c r="P9" s="1">
-        <v>0.86186481663692605</v>
-      </c>
       <c r="Q9">
-        <v>390.1</v>
+        <v>258.39999999999998</v>
       </c>
       <c r="R9">
         <v>299</v>
       </c>
-      <c r="S9">
+      <c r="W9">
+        <v>390.1</v>
+      </c>
+      <c r="X9">
+        <v>299</v>
+      </c>
+      <c r="Y9">
         <v>44.5</v>
       </c>
-      <c r="T9">
+      <c r="Z9">
         <v>860</v>
       </c>
-      <c r="U9" s="1">
+      <c r="AA9" s="1">
         <v>5.4866666666666601</v>
       </c>
-      <c r="V9" s="1">
+      <c r="AB9" s="1">
         <v>1.3037883725205099</v>
       </c>
-      <c r="W9" s="2">
+      <c r="AC9" s="2">
         <v>13.81090605</v>
       </c>
-      <c r="X9" s="2">
-        <v>13.31891891891892</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2012</v>
       </c>
@@ -5255,56 +5435,53 @@
       <c r="H10">
         <v>58</v>
       </c>
-      <c r="I10">
-        <v>352.1</v>
-      </c>
-      <c r="J10">
-        <v>322</v>
-      </c>
       <c r="K10">
         <v>2012</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10">
+        <v>43.3</v>
+      </c>
+      <c r="M10">
+        <v>1009</v>
+      </c>
+      <c r="N10" s="1">
+        <v>4.62</v>
+      </c>
+      <c r="O10" s="1">
+        <v>1.0901097540209601</v>
+      </c>
+      <c r="P10" s="2">
         <v>15.135</v>
       </c>
-      <c r="M10">
-        <v>43.3</v>
-      </c>
-      <c r="N10">
-        <v>1009</v>
-      </c>
-      <c r="O10" s="1">
-        <v>4.62</v>
-      </c>
-      <c r="P10" s="1">
-        <v>1.0901097540209601</v>
-      </c>
       <c r="Q10">
+        <v>352.1</v>
+      </c>
+      <c r="R10">
+        <v>322</v>
+      </c>
+      <c r="W10">
         <v>282.7</v>
       </c>
-      <c r="R10">
+      <c r="X10">
         <v>301</v>
       </c>
-      <c r="S10">
+      <c r="Y10">
         <v>41.3</v>
       </c>
-      <c r="T10">
+      <c r="Z10">
         <v>957</v>
       </c>
-      <c r="U10" s="1">
+      <c r="AA10" s="1">
         <v>3.91333333333333</v>
       </c>
-      <c r="V10" s="1">
+      <c r="AB10" s="1">
         <v>0.93909346089325096</v>
       </c>
-      <c r="W10" s="2">
+      <c r="AC10" s="2">
         <v>12.40419234</v>
       </c>
-      <c r="X10" s="2">
-        <v>15.135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2011</v>
       </c>
@@ -5329,56 +5506,53 @@
       <c r="H11">
         <v>60</v>
       </c>
-      <c r="I11">
-        <v>281.2</v>
-      </c>
-      <c r="J11">
-        <v>300</v>
-      </c>
       <c r="K11">
         <v>2011</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11">
+        <v>44.3</v>
+      </c>
+      <c r="M11">
+        <v>999</v>
+      </c>
+      <c r="N11" s="1">
+        <v>4.3333333333333304</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0.93600732295914102</v>
+      </c>
+      <c r="P11" s="2">
         <v>12.588888888888889</v>
       </c>
-      <c r="M11">
-        <v>44.3</v>
-      </c>
-      <c r="N11">
-        <v>999</v>
-      </c>
-      <c r="O11" s="1">
-        <v>4.3333333333333304</v>
-      </c>
-      <c r="P11" s="1">
-        <v>0.93600732295914102</v>
-      </c>
       <c r="Q11">
+        <v>281.2</v>
+      </c>
+      <c r="R11">
+        <v>300</v>
+      </c>
+      <c r="W11">
         <v>315</v>
       </c>
-      <c r="R11">
+      <c r="X11">
         <v>301</v>
       </c>
-      <c r="S11">
+      <c r="Y11">
         <v>40</v>
       </c>
-      <c r="T11">
+      <c r="Z11">
         <v>967</v>
       </c>
-      <c r="U11" s="1">
+      <c r="AA11" s="1">
         <v>5.17</v>
       </c>
-      <c r="V11" s="1">
+      <c r="AB11" s="1">
         <v>1.0463899546564299</v>
       </c>
-      <c r="W11" s="2">
+      <c r="AC11" s="2">
         <v>12.980670249999999</v>
       </c>
-      <c r="X11" s="2">
-        <v>12.588888888888889</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2009</v>
       </c>
@@ -5403,56 +5577,53 @@
       <c r="H12">
         <v>64</v>
       </c>
-      <c r="I12">
-        <v>221.6</v>
-      </c>
-      <c r="J12">
-        <v>290</v>
-      </c>
       <c r="K12">
-        <v>2009</v>
-      </c>
-      <c r="L12" s="2">
-        <v>12.28</v>
+        <v>2010</v>
+      </c>
+      <c r="L12">
+        <v>42.9</v>
       </c>
       <c r="M12">
-        <v>39.9</v>
-      </c>
-      <c r="N12">
-        <v>954</v>
+        <v>1048</v>
+      </c>
+      <c r="N12" s="1">
+        <v>5.7066666666666599</v>
       </c>
       <c r="O12" s="1">
-        <v>5.0699999999999896</v>
-      </c>
-      <c r="P12" s="1">
-        <v>0.76159054198027298</v>
+        <v>0.72820467500331398</v>
+      </c>
+      <c r="P12" s="2">
+        <v>13.95</v>
       </c>
       <c r="Q12">
+        <v>247.2</v>
+      </c>
+      <c r="R12">
+        <v>339</v>
+      </c>
+      <c r="W12">
         <v>258.39999999999998</v>
       </c>
-      <c r="R12">
+      <c r="X12">
         <v>299</v>
       </c>
-      <c r="S12">
+      <c r="Y12">
         <v>43.8</v>
       </c>
-      <c r="T12">
+      <c r="Z12">
         <v>911</v>
       </c>
-      <c r="U12" s="1">
+      <c r="AA12" s="1">
         <v>3.44</v>
       </c>
-      <c r="V12" s="1">
+      <c r="AB12" s="1">
         <v>0.86186481663692605</v>
       </c>
-      <c r="W12" s="2">
+      <c r="AC12" s="2">
         <v>11.972047160000001</v>
       </c>
-      <c r="X12" s="2">
-        <v>12.28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2008</v>
       </c>
@@ -5477,56 +5648,53 @@
       <c r="H13">
         <v>62</v>
       </c>
-      <c r="I13">
-        <v>253.8</v>
-      </c>
-      <c r="J13">
-        <v>286</v>
-      </c>
       <c r="K13">
-        <v>2008</v>
-      </c>
-      <c r="L13" s="2">
-        <v>12.725</v>
+        <v>2009</v>
+      </c>
+      <c r="L13">
+        <v>39.9</v>
       </c>
       <c r="M13">
-        <v>39.1</v>
-      </c>
-      <c r="N13">
-        <v>912</v>
+        <v>954</v>
+      </c>
+      <c r="N13" s="1">
+        <v>5.0699999999999896</v>
       </c>
       <c r="O13" s="1">
-        <v>6.0333333333333297</v>
-      </c>
-      <c r="P13" s="1">
-        <v>0.88524590163934402</v>
+        <v>0.76159054198027298</v>
+      </c>
+      <c r="P13" s="2">
+        <v>12.28</v>
       </c>
       <c r="Q13">
+        <v>221.6</v>
+      </c>
+      <c r="R13">
+        <v>290</v>
+      </c>
+      <c r="W13">
         <v>352.1</v>
       </c>
-      <c r="R13">
+      <c r="X13">
         <v>322</v>
       </c>
-      <c r="S13">
+      <c r="Y13">
         <v>43.3</v>
       </c>
-      <c r="T13">
+      <c r="Z13">
         <v>1009</v>
       </c>
-      <c r="U13" s="1">
+      <c r="AA13" s="1">
         <v>4.62</v>
       </c>
-      <c r="V13" s="1">
+      <c r="AB13" s="1">
         <v>1.0901097540209601</v>
       </c>
-      <c r="W13" s="2">
+      <c r="AC13" s="2">
         <v>11.57489485</v>
       </c>
-      <c r="X13" s="2">
-        <v>12.725</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2006</v>
       </c>
@@ -5551,57 +5719,53 @@
       <c r="H14">
         <v>63</v>
       </c>
-      <c r="I14">
-        <v>366.1</v>
-      </c>
-      <c r="J14">
-        <v>284</v>
-      </c>
       <c r="K14">
-        <v>2006</v>
-      </c>
-      <c r="L14" s="2">
-        <v>13.112500000000001</v>
+        <v>2008</v>
+      </c>
+      <c r="L14">
+        <v>39.1</v>
       </c>
       <c r="M14">
-        <v>39.5</v>
-      </c>
-      <c r="N14">
-        <v>947</v>
+        <v>912</v>
+      </c>
+      <c r="N14" s="1">
+        <v>6.0333333333333297</v>
       </c>
       <c r="O14" s="1">
-        <v>5.3466666666666596</v>
-      </c>
-      <c r="P14" s="1">
-        <v>1.28514761119106</v>
+        <v>0.88524590163934402</v>
+      </c>
+      <c r="P14" s="2">
+        <v>12.725</v>
       </c>
       <c r="Q14">
+        <v>253.8</v>
+      </c>
+      <c r="R14">
+        <v>286</v>
+      </c>
+      <c r="W14">
         <v>281.2</v>
       </c>
-      <c r="R14">
+      <c r="X14">
         <v>300</v>
       </c>
-      <c r="S14">
+      <c r="Y14">
         <v>44.3</v>
       </c>
-      <c r="T14">
+      <c r="Z14">
         <v>999</v>
       </c>
-      <c r="U14" s="1">
+      <c r="AA14" s="1">
         <v>4.3333333333333304</v>
       </c>
-      <c r="V14" s="1">
+      <c r="AB14" s="1">
         <v>0.93600732295914102</v>
       </c>
-      <c r="W14" s="2">
+      <c r="AC14" s="2">
         <v>12.529942569999999</v>
       </c>
-      <c r="X14" s="2">
-        <v>13.112500000000001</v>
-      </c>
-      <c r="Z14" s="3"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2005</v>
       </c>
@@ -5626,56 +5790,53 @@
       <c r="H15">
         <v>56</v>
       </c>
-      <c r="I15">
-        <v>293.39999999999998</v>
-      </c>
-      <c r="J15">
-        <v>295</v>
-      </c>
       <c r="K15">
-        <v>2005</v>
-      </c>
-      <c r="L15" s="2">
-        <v>13.309090909090909</v>
+        <v>2006</v>
+      </c>
+      <c r="L15">
+        <v>39.5</v>
       </c>
       <c r="M15">
-        <v>41.3</v>
-      </c>
-      <c r="N15">
-        <v>965</v>
+        <v>947</v>
+      </c>
+      <c r="N15" s="1">
+        <v>5.3466666666666596</v>
       </c>
       <c r="O15" s="1">
-        <v>4.2033333333333296</v>
-      </c>
-      <c r="P15" s="1">
-        <v>0.99376778214334105</v>
+        <v>1.28514761119106</v>
+      </c>
+      <c r="P15" s="2">
+        <v>13.112500000000001</v>
       </c>
       <c r="Q15">
+        <v>366.1</v>
+      </c>
+      <c r="R15">
+        <v>284</v>
+      </c>
+      <c r="W15">
         <v>247.2</v>
       </c>
-      <c r="R15">
+      <c r="X15">
         <v>339</v>
       </c>
-      <c r="S15">
+      <c r="Y15">
         <v>42.9</v>
       </c>
-      <c r="T15">
+      <c r="Z15">
         <v>1048</v>
       </c>
-      <c r="U15" s="1">
+      <c r="AA15" s="1">
         <v>5.7066666666666599</v>
       </c>
-      <c r="V15" s="1">
+      <c r="AB15" s="1">
         <v>0.72820467500331398</v>
       </c>
-      <c r="W15" s="2">
+      <c r="AC15" s="2">
         <v>12.966400200000001</v>
       </c>
-      <c r="X15" s="2">
-        <v>13.309090909090909</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F16">
         <v>2009</v>
       </c>
@@ -5685,56 +5846,53 @@
       <c r="H16">
         <v>59</v>
       </c>
-      <c r="I16">
-        <v>554</v>
-      </c>
-      <c r="J16">
-        <v>263</v>
-      </c>
       <c r="K16">
-        <v>2004</v>
-      </c>
-      <c r="L16" s="2">
-        <v>11.176923076923078</v>
+        <v>2005</v>
+      </c>
+      <c r="L16">
+        <v>41.3</v>
       </c>
       <c r="M16">
-        <v>39.799999999999997</v>
-      </c>
-      <c r="N16">
-        <v>787</v>
+        <v>965</v>
+      </c>
+      <c r="N16" s="1">
+        <v>4.2033333333333296</v>
       </c>
       <c r="O16" s="1">
-        <v>5.5133333333333301</v>
-      </c>
-      <c r="P16" s="1">
-        <v>2.10344565877352</v>
+        <v>0.99376778214334105</v>
+      </c>
+      <c r="P16" s="2">
+        <v>13.309090909090909</v>
       </c>
       <c r="Q16">
+        <v>293.39999999999998</v>
+      </c>
+      <c r="R16">
+        <v>295</v>
+      </c>
+      <c r="W16">
         <v>221.6</v>
       </c>
-      <c r="R16">
+      <c r="X16">
         <v>290</v>
       </c>
-      <c r="S16">
+      <c r="Y16">
         <v>39.9</v>
       </c>
-      <c r="T16">
+      <c r="Z16">
         <v>954</v>
       </c>
-      <c r="U16" s="1">
+      <c r="AA16" s="1">
         <v>5.0699999999999896</v>
       </c>
-      <c r="V16" s="1">
+      <c r="AB16" s="1">
         <v>0.76159054198027298</v>
       </c>
-      <c r="W16" s="2">
+      <c r="AC16" s="2">
         <v>12.04823423</v>
       </c>
-      <c r="X16" s="2">
-        <v>11.176923076923078</v>
-      </c>
-    </row>
-    <row r="17" spans="4:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="4:29" x14ac:dyDescent="0.25">
       <c r="F17">
         <v>2008</v>
       </c>
@@ -5744,56 +5902,53 @@
       <c r="H17">
         <v>65</v>
       </c>
-      <c r="I17">
-        <v>349.7</v>
-      </c>
-      <c r="J17">
-        <v>268</v>
-      </c>
       <c r="K17">
-        <v>2003</v>
-      </c>
-      <c r="L17" s="2">
-        <v>15.042857142857141</v>
+        <v>2004</v>
+      </c>
+      <c r="L17">
+        <v>39.799999999999997</v>
       </c>
       <c r="M17">
-        <v>38.799999999999997</v>
-      </c>
-      <c r="N17">
-        <v>917</v>
+        <v>787</v>
+      </c>
+      <c r="N17" s="1">
+        <v>5.5133333333333301</v>
       </c>
       <c r="O17" s="1">
-        <v>3.67</v>
-      </c>
-      <c r="P17" s="1">
-        <v>1.3014272157198401</v>
+        <v>2.10344565877352</v>
+      </c>
+      <c r="P17" s="2">
+        <v>11.176923076923078</v>
       </c>
       <c r="Q17">
+        <v>554</v>
+      </c>
+      <c r="R17">
+        <v>263</v>
+      </c>
+      <c r="W17">
         <v>253.8</v>
       </c>
-      <c r="R17">
+      <c r="X17">
         <v>286</v>
       </c>
-      <c r="S17">
+      <c r="Y17">
         <v>39.1</v>
       </c>
-      <c r="T17">
+      <c r="Z17">
         <v>912</v>
       </c>
-      <c r="U17" s="1">
+      <c r="AA17" s="1">
         <v>6.0333333333333297</v>
       </c>
-      <c r="V17" s="1">
+      <c r="AB17" s="1">
         <v>0.88524590163934402</v>
       </c>
-      <c r="W17" s="2">
+      <c r="AC17" s="2">
         <v>13.898573499999999</v>
       </c>
-      <c r="X17" s="2">
-        <v>15.042857142857141</v>
-      </c>
-    </row>
-    <row r="18" spans="4:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="4:29" x14ac:dyDescent="0.25">
       <c r="F18">
         <v>2007</v>
       </c>
@@ -5803,56 +5958,53 @@
       <c r="H18">
         <v>68</v>
       </c>
-      <c r="I18">
-        <v>426</v>
-      </c>
-      <c r="J18">
-        <v>297</v>
-      </c>
       <c r="K18">
-        <v>2002</v>
-      </c>
-      <c r="L18" s="2">
-        <v>12.1</v>
+        <v>2003</v>
+      </c>
+      <c r="L18">
+        <v>38.799999999999997</v>
       </c>
       <c r="M18">
-        <v>40.4</v>
-      </c>
-      <c r="N18">
-        <v>1033</v>
+        <v>917</v>
+      </c>
+      <c r="N18" s="1">
+        <v>3.67</v>
       </c>
       <c r="O18" s="1">
-        <v>4.87</v>
-      </c>
-      <c r="P18" s="1">
-        <v>1.4353519372538399</v>
+        <v>1.3014272157198401</v>
+      </c>
+      <c r="P18" s="2">
+        <v>15.042857142857141</v>
       </c>
       <c r="Q18">
+        <v>349.7</v>
+      </c>
+      <c r="R18">
+        <v>268</v>
+      </c>
+      <c r="W18">
         <v>342.4</v>
       </c>
-      <c r="R18">
+      <c r="X18">
         <v>301</v>
       </c>
-      <c r="S18">
+      <c r="Y18">
         <v>41.599999999999902</v>
       </c>
-      <c r="T18">
+      <c r="Z18">
         <v>1020</v>
       </c>
-      <c r="U18" s="1">
+      <c r="AA18" s="1">
         <v>4.2966666666666598</v>
       </c>
-      <c r="V18" s="1">
+      <c r="AB18" s="1">
         <v>1.1362580473883299</v>
       </c>
-      <c r="W18" s="2">
+      <c r="AC18" s="2">
         <v>12.848453109999999</v>
       </c>
-      <c r="X18" s="2">
-        <v>12.1</v>
-      </c>
-    </row>
-    <row r="19" spans="4:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="4:29" x14ac:dyDescent="0.25">
       <c r="F19">
         <v>2006</v>
       </c>
@@ -5862,56 +6014,53 @@
       <c r="H19">
         <v>71</v>
       </c>
-      <c r="I19">
-        <v>370</v>
-      </c>
-      <c r="J19">
-        <v>293</v>
-      </c>
       <c r="K19">
-        <v>2001</v>
-      </c>
-      <c r="L19" s="2">
-        <v>12.532142857142857</v>
+        <v>2002</v>
+      </c>
+      <c r="L19">
+        <v>40.4</v>
       </c>
       <c r="M19">
-        <v>42</v>
-      </c>
-      <c r="N19">
-        <v>913</v>
+        <v>1033</v>
+      </c>
+      <c r="N19" s="1">
+        <v>4.87</v>
       </c>
       <c r="O19" s="1">
-        <v>4.0033333333333303</v>
-      </c>
-      <c r="P19" s="1">
-        <v>1.2647344808174501</v>
+        <v>1.4353519372538399</v>
+      </c>
+      <c r="P19" s="2">
+        <v>12.1</v>
       </c>
       <c r="Q19">
+        <v>426</v>
+      </c>
+      <c r="R19">
+        <v>297</v>
+      </c>
+      <c r="W19">
         <v>366.1</v>
       </c>
-      <c r="R19">
+      <c r="X19">
         <v>284</v>
       </c>
-      <c r="S19">
+      <c r="Y19">
         <v>39.5</v>
       </c>
-      <c r="T19">
+      <c r="Z19">
         <v>947</v>
       </c>
-      <c r="U19" s="1">
+      <c r="AA19" s="1">
         <v>5.3466666666666596</v>
       </c>
-      <c r="V19" s="1">
+      <c r="AB19" s="1">
         <v>1.28514761119106</v>
       </c>
-      <c r="W19" s="2">
+      <c r="AC19" s="2">
         <v>13.89854016</v>
       </c>
-      <c r="X19" s="2">
-        <v>12.532142857142857</v>
-      </c>
-    </row>
-    <row r="20" spans="4:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="4:29" x14ac:dyDescent="0.25">
       <c r="F20">
         <v>2005</v>
       </c>
@@ -5921,467 +6070,497 @@
       <c r="H20">
         <v>68</v>
       </c>
-      <c r="I20">
+      <c r="K20">
+        <v>2001</v>
+      </c>
+      <c r="L20">
+        <v>42</v>
+      </c>
+      <c r="M20">
+        <v>913</v>
+      </c>
+      <c r="N20" s="1">
+        <v>4.0033333333333303</v>
+      </c>
+      <c r="O20" s="1">
+        <v>1.2647344808174501</v>
+      </c>
+      <c r="P20" s="2">
+        <v>12.532142857142857</v>
+      </c>
+      <c r="Q20">
+        <v>370</v>
+      </c>
+      <c r="R20">
+        <v>293</v>
+      </c>
+      <c r="W20">
+        <v>293.39999999999998</v>
+      </c>
+      <c r="X20">
+        <v>295</v>
+      </c>
+      <c r="Y20">
+        <v>41.3</v>
+      </c>
+      <c r="Z20">
+        <v>965</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>4.2033333333333296</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>0.99376778214334105</v>
+      </c>
+      <c r="AC20" s="2">
+        <v>12.9389074</v>
+      </c>
+    </row>
+    <row r="21" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <v>2000</v>
+      </c>
+      <c r="L21">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="M21">
+        <v>835</v>
+      </c>
+      <c r="N21" s="1">
+        <v>5.1766666666666596</v>
+      </c>
+      <c r="O21" s="1">
+        <v>1.5003135357878701</v>
+      </c>
+      <c r="P21" s="2">
+        <v>14.05</v>
+      </c>
+      <c r="Q21">
         <v>418</v>
       </c>
-      <c r="J20">
+      <c r="R21">
         <v>279</v>
       </c>
-      <c r="K20">
-        <v>2000</v>
-      </c>
-      <c r="L20" s="2">
-        <v>14.05</v>
-      </c>
-      <c r="M20">
+      <c r="W21">
+        <v>554</v>
+      </c>
+      <c r="X21">
+        <v>263</v>
+      </c>
+      <c r="Y21">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="Z21">
+        <v>787</v>
+      </c>
+      <c r="AA21" s="1">
+        <v>5.5133333333333301</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>2.10344565877352</v>
+      </c>
+      <c r="AC21" s="2">
+        <v>11.98232353</v>
+      </c>
+    </row>
+    <row r="22" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>1999</v>
+      </c>
+      <c r="L22">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="M22">
+        <v>946</v>
+      </c>
+      <c r="N22" s="1">
+        <v>4.1133333333333297</v>
+      </c>
+      <c r="O22" s="1">
+        <v>0.72903769005992702</v>
+      </c>
+      <c r="P22" s="2">
+        <v>11.8</v>
+      </c>
+      <c r="Q22">
+        <v>220</v>
+      </c>
+      <c r="R22">
+        <v>302</v>
+      </c>
+      <c r="W22">
+        <v>349.7</v>
+      </c>
+      <c r="X22">
+        <v>268</v>
+      </c>
+      <c r="Y22">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="Z22">
+        <v>917</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>3.67</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>1.3014272157198401</v>
+      </c>
+      <c r="AC22" s="2">
+        <v>13.413161710000001</v>
+      </c>
+    </row>
+    <row r="23" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <v>1998</v>
+      </c>
+      <c r="L23">
+        <v>40.4</v>
+      </c>
+      <c r="M23">
+        <v>982</v>
+      </c>
+      <c r="N23" s="1">
+        <v>5.3066666666666604</v>
+      </c>
+      <c r="O23" s="1">
+        <v>0.93681729826432403</v>
+      </c>
+      <c r="P23" s="2">
+        <v>12.37142857142857</v>
+      </c>
+      <c r="Q23">
+        <v>272</v>
+      </c>
+      <c r="R23">
+        <v>290</v>
+      </c>
+      <c r="W23">
+        <v>426</v>
+      </c>
+      <c r="X23">
+        <v>297</v>
+      </c>
+      <c r="Y23">
+        <v>40.4</v>
+      </c>
+      <c r="Z23">
+        <v>1033</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>4.87</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>1.4353519372538399</v>
+      </c>
+      <c r="AC23" s="2">
+        <v>12.67487704</v>
+      </c>
+    </row>
+    <row r="24" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="D24" s="2"/>
+      <c r="K24">
+        <v>1997</v>
+      </c>
+      <c r="L24">
+        <v>42.6</v>
+      </c>
+      <c r="M24">
+        <v>863</v>
+      </c>
+      <c r="N24" s="1">
+        <v>3.7466666666666599</v>
+      </c>
+      <c r="O24" s="1">
+        <v>1.92939708777606</v>
+      </c>
+      <c r="P24" s="2">
+        <v>14.416666666666666</v>
+      </c>
+      <c r="Q24">
+        <v>494</v>
+      </c>
+      <c r="R24">
+        <v>256</v>
+      </c>
+      <c r="W24">
+        <v>370</v>
+      </c>
+      <c r="X24">
+        <v>293</v>
+      </c>
+      <c r="Y24">
+        <v>42</v>
+      </c>
+      <c r="Z24">
+        <v>913</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>4.0033333333333303</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>1.2647344808174501</v>
+      </c>
+      <c r="AC24" s="2">
+        <v>12.493339020000001</v>
+      </c>
+    </row>
+    <row r="25" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="D25" s="2"/>
+      <c r="K25">
+        <v>1996</v>
+      </c>
+      <c r="L25">
+        <v>41</v>
+      </c>
+      <c r="M25">
+        <v>976</v>
+      </c>
+      <c r="N25" s="1">
+        <v>5.3866666666666596</v>
+      </c>
+      <c r="O25" s="1">
+        <v>1.4126870990734099</v>
+      </c>
+      <c r="P25" s="2">
+        <v>12.55</v>
+      </c>
+      <c r="Q25">
+        <v>396</v>
+      </c>
+      <c r="R25">
+        <v>280</v>
+      </c>
+      <c r="W25">
+        <v>418</v>
+      </c>
+      <c r="X25">
+        <v>279</v>
+      </c>
+      <c r="Y25">
         <v>39.200000000000003</v>
       </c>
-      <c r="N20">
+      <c r="Z25">
         <v>835</v>
       </c>
-      <c r="O20" s="1">
+      <c r="AA25" s="1">
         <v>5.1766666666666596</v>
       </c>
-      <c r="P20" s="1">
+      <c r="AB25" s="1">
         <v>1.5003135357878701</v>
       </c>
-      <c r="Q20">
-        <v>293.39999999999998</v>
-      </c>
-      <c r="R20">
-        <v>295</v>
-      </c>
-      <c r="S20">
-        <v>41.3</v>
-      </c>
-      <c r="T20">
-        <v>965</v>
-      </c>
-      <c r="U20" s="1">
+      <c r="AC25" s="2">
+        <v>12.2148875</v>
+      </c>
+    </row>
+    <row r="26" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="D26" s="2"/>
+      <c r="K26">
+        <v>1993</v>
+      </c>
+      <c r="L26">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="M26">
+        <v>837</v>
+      </c>
+      <c r="N26" s="1">
         <v>4.2033333333333296</v>
       </c>
-      <c r="V20" s="1">
-        <v>0.99376778214334105</v>
-      </c>
-      <c r="W20" s="2">
-        <v>12.9389074</v>
-      </c>
-      <c r="X20" s="2">
-        <v>14.05</v>
-      </c>
-    </row>
-    <row r="21" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="I21">
+      <c r="O26" s="1">
+        <v>1.63526629149335</v>
+      </c>
+      <c r="P26" s="2">
+        <v>12.01</v>
+      </c>
+      <c r="Q26">
+        <v>401</v>
+      </c>
+      <c r="R26">
+        <v>245</v>
+      </c>
+      <c r="W26">
+        <v>220</v>
+      </c>
+      <c r="X26">
+        <v>302</v>
+      </c>
+      <c r="Y26">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="Z26">
+        <v>946</v>
+      </c>
+      <c r="AA26" s="1">
+        <v>4.1133333333333297</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>0.72903769005992702</v>
+      </c>
+    </row>
+    <row r="27" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="D27" s="2"/>
+      <c r="K27">
+        <v>1992</v>
+      </c>
+      <c r="L27">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="M27">
+        <v>734</v>
+      </c>
+      <c r="N27" s="1">
+        <v>5.6866666666666603</v>
+      </c>
+      <c r="O27" s="1">
+        <v>1.2822816079047801</v>
+      </c>
+      <c r="P27" s="2">
+        <v>12.753846153846153</v>
+      </c>
+      <c r="Q27">
+        <v>342</v>
+      </c>
+      <c r="R27">
+        <v>267</v>
+      </c>
+      <c r="W27">
         <v>272</v>
       </c>
-      <c r="J21">
+      <c r="X27">
         <v>290</v>
       </c>
-      <c r="K21">
-        <v>1998</v>
-      </c>
-      <c r="L21" s="2">
-        <v>12.37142857142857</v>
-      </c>
-      <c r="M21">
+      <c r="Y27">
         <v>40.4</v>
       </c>
-      <c r="N21">
+      <c r="Z27">
         <v>982</v>
       </c>
-      <c r="O21" s="1">
+      <c r="AA27" s="1">
         <v>5.3066666666666604</v>
       </c>
-      <c r="P21" s="1">
+      <c r="AB27" s="1">
         <v>0.93681729826432403</v>
       </c>
-      <c r="Q21">
-        <v>554</v>
-      </c>
-      <c r="R21">
-        <v>263</v>
-      </c>
-      <c r="S21">
-        <v>39.799999999999997</v>
-      </c>
-      <c r="T21">
-        <v>787</v>
-      </c>
-      <c r="U21" s="1">
-        <v>5.5133333333333301</v>
-      </c>
-      <c r="V21" s="1">
-        <v>2.10344565877352</v>
-      </c>
-      <c r="W21" s="2">
-        <v>11.98232353</v>
-      </c>
-      <c r="X21" s="2">
-        <v>12.37142857142857</v>
-      </c>
-    </row>
-    <row r="22" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="I22">
+    </row>
+    <row r="28" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="D28" s="2"/>
+      <c r="W28">
         <v>494</v>
       </c>
-      <c r="J22">
+      <c r="X28">
         <v>256</v>
       </c>
-      <c r="K22">
-        <v>1997</v>
-      </c>
-      <c r="L22" s="2">
-        <v>14.416666666666666</v>
-      </c>
-      <c r="M22">
+      <c r="Y28">
         <v>42.6</v>
       </c>
-      <c r="N22">
+      <c r="Z28">
         <v>863</v>
       </c>
-      <c r="O22" s="1">
+      <c r="AA28" s="1">
         <v>3.7466666666666599</v>
       </c>
-      <c r="P22" s="1">
+      <c r="AB28" s="1">
         <v>1.92939708777606</v>
       </c>
-      <c r="Q22">
-        <v>349.7</v>
-      </c>
-      <c r="R22">
-        <v>268</v>
-      </c>
-      <c r="S22">
-        <v>38.799999999999997</v>
-      </c>
-      <c r="T22">
-        <v>917</v>
-      </c>
-      <c r="U22" s="1">
-        <v>3.67</v>
-      </c>
-      <c r="V22" s="1">
-        <v>1.3014272157198401</v>
-      </c>
-      <c r="W22" s="2">
-        <v>13.413161710000001</v>
-      </c>
-      <c r="X22" s="2">
-        <v>14.416666666666666</v>
-      </c>
-    </row>
-    <row r="23" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="I23">
+    </row>
+    <row r="29" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="W29">
         <v>396</v>
       </c>
-      <c r="J23">
+      <c r="X29">
         <v>280</v>
       </c>
-      <c r="K23">
-        <v>1996</v>
-      </c>
-      <c r="L23" s="2">
-        <v>12.55</v>
-      </c>
-      <c r="M23">
+      <c r="Y29">
         <v>41</v>
       </c>
-      <c r="N23">
+      <c r="Z29">
         <v>976</v>
       </c>
-      <c r="O23" s="1">
+      <c r="AA29" s="1">
         <v>5.3866666666666596</v>
       </c>
-      <c r="P23" s="1">
+      <c r="AB29" s="1">
         <v>1.4126870990734099</v>
       </c>
-      <c r="Q23">
-        <v>426</v>
-      </c>
-      <c r="R23">
-        <v>297</v>
-      </c>
-      <c r="S23">
-        <v>40.4</v>
-      </c>
-      <c r="T23">
-        <v>1033</v>
-      </c>
-      <c r="U23" s="1">
-        <v>4.87</v>
-      </c>
-      <c r="V23" s="1">
-        <v>1.4353519372538399</v>
-      </c>
-      <c r="W23" s="2">
-        <v>12.67487704</v>
-      </c>
-      <c r="X23" s="2">
-        <v>12.55</v>
-      </c>
-    </row>
-    <row r="24" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="D24" s="2"/>
-      <c r="I24">
+    </row>
+    <row r="30" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="W30">
+        <v>346.3</v>
+      </c>
+      <c r="X30">
+        <v>291</v>
+      </c>
+      <c r="Y30">
+        <v>39.699999999999903</v>
+      </c>
+      <c r="Z30">
+        <v>918</v>
+      </c>
+      <c r="AA30" s="1">
+        <v>2.9866666666666601</v>
+      </c>
+      <c r="AB30" s="1">
+        <v>1.19015706086538</v>
+      </c>
+    </row>
+    <row r="31" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="W31">
+        <v>216.9</v>
+      </c>
+      <c r="X31">
+        <v>279</v>
+      </c>
+      <c r="Y31">
+        <v>36.9</v>
+      </c>
+      <c r="Z31">
+        <v>804</v>
+      </c>
+      <c r="AA31" s="1">
+        <v>4.6266666666666598</v>
+      </c>
+      <c r="AB31" s="1">
+        <v>0.77636194430524696</v>
+      </c>
+    </row>
+    <row r="32" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="W32">
         <v>401</v>
       </c>
-      <c r="J24">
+      <c r="X32">
         <v>245</v>
       </c>
-      <c r="K24">
-        <v>1993</v>
-      </c>
-      <c r="L24" s="2">
-        <v>12.01</v>
-      </c>
-      <c r="M24">
+      <c r="Y32">
         <v>37.299999999999997</v>
       </c>
-      <c r="N24">
+      <c r="Z32">
         <v>837</v>
       </c>
-      <c r="O24" s="1">
+      <c r="AA32" s="1">
         <v>4.2033333333333296</v>
       </c>
-      <c r="P24" s="1">
+      <c r="AB32" s="1">
         <v>1.63526629149335</v>
       </c>
-      <c r="Q24">
-        <v>370</v>
-      </c>
-      <c r="R24">
-        <v>293</v>
-      </c>
-      <c r="S24">
-        <v>42</v>
-      </c>
-      <c r="T24">
-        <v>913</v>
-      </c>
-      <c r="U24" s="1">
-        <v>4.0033333333333303</v>
-      </c>
-      <c r="V24" s="1">
-        <v>1.2647344808174501</v>
-      </c>
-      <c r="W24" s="2">
-        <v>12.493339020000001</v>
-      </c>
-      <c r="X24" s="2">
-        <v>12.01</v>
-      </c>
-    </row>
-    <row r="25" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="D25" s="2"/>
-      <c r="I25">
+    </row>
+    <row r="33" spans="23:28" x14ac:dyDescent="0.25">
+      <c r="W33">
         <v>342</v>
       </c>
-      <c r="J25">
+      <c r="X33">
         <v>267</v>
       </c>
-      <c r="K25">
-        <v>1992</v>
-      </c>
-      <c r="L25" s="2">
-        <v>12.753846153846153</v>
-      </c>
-      <c r="M25">
+      <c r="Y33">
         <v>35.200000000000003</v>
       </c>
-      <c r="N25">
+      <c r="Z33">
         <v>734</v>
       </c>
-      <c r="O25" s="1">
+      <c r="AA33" s="1">
         <v>5.6866666666666603</v>
       </c>
-      <c r="P25" s="1">
-        <v>1.2822816079047801</v>
-      </c>
-      <c r="Q25">
-        <v>418</v>
-      </c>
-      <c r="R25">
-        <v>279</v>
-      </c>
-      <c r="S25">
-        <v>39.200000000000003</v>
-      </c>
-      <c r="T25">
-        <v>835</v>
-      </c>
-      <c r="U25" s="1">
-        <v>5.1766666666666596</v>
-      </c>
-      <c r="V25" s="1">
-        <v>1.5003135357878701</v>
-      </c>
-      <c r="W25" s="2">
-        <v>12.2148875</v>
-      </c>
-      <c r="X25" s="2">
-        <v>12.753846153846153</v>
-      </c>
-    </row>
-    <row r="26" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="D26" s="2"/>
-      <c r="Q26">
-        <v>220</v>
-      </c>
-      <c r="R26">
-        <v>302</v>
-      </c>
-      <c r="S26">
-        <v>39.799999999999997</v>
-      </c>
-      <c r="T26">
-        <v>946</v>
-      </c>
-      <c r="U26" s="1">
-        <v>4.1133333333333297</v>
-      </c>
-      <c r="V26" s="1">
-        <v>0.72903769005992702</v>
-      </c>
-    </row>
-    <row r="27" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="D27" s="2"/>
-      <c r="Q27">
-        <v>272</v>
-      </c>
-      <c r="R27">
-        <v>290</v>
-      </c>
-      <c r="S27">
-        <v>40.4</v>
-      </c>
-      <c r="T27">
-        <v>982</v>
-      </c>
-      <c r="U27" s="1">
-        <v>5.3066666666666604</v>
-      </c>
-      <c r="V27" s="1">
-        <v>0.93681729826432403</v>
-      </c>
-    </row>
-    <row r="28" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="D28" s="2"/>
-      <c r="Q28">
-        <v>494</v>
-      </c>
-      <c r="R28">
-        <v>256</v>
-      </c>
-      <c r="S28">
-        <v>42.6</v>
-      </c>
-      <c r="T28">
-        <v>863</v>
-      </c>
-      <c r="U28" s="1">
-        <v>3.7466666666666599</v>
-      </c>
-      <c r="V28" s="1">
-        <v>1.92939708777606</v>
-      </c>
-    </row>
-    <row r="29" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="Q29">
-        <v>396</v>
-      </c>
-      <c r="R29">
-        <v>280</v>
-      </c>
-      <c r="S29">
-        <v>41</v>
-      </c>
-      <c r="T29">
-        <v>976</v>
-      </c>
-      <c r="U29" s="1">
-        <v>5.3866666666666596</v>
-      </c>
-      <c r="V29" s="1">
-        <v>1.4126870990734099</v>
-      </c>
-    </row>
-    <row r="30" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="Q30">
-        <v>346.3</v>
-      </c>
-      <c r="R30">
-        <v>291</v>
-      </c>
-      <c r="S30">
-        <v>39.699999999999903</v>
-      </c>
-      <c r="T30">
-        <v>918</v>
-      </c>
-      <c r="U30" s="1">
-        <v>2.9866666666666601</v>
-      </c>
-      <c r="V30" s="1">
-        <v>1.19015706086538</v>
-      </c>
-    </row>
-    <row r="31" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="Q31">
-        <v>216.9</v>
-      </c>
-      <c r="R31">
-        <v>279</v>
-      </c>
-      <c r="S31">
-        <v>36.9</v>
-      </c>
-      <c r="T31">
-        <v>804</v>
-      </c>
-      <c r="U31" s="1">
-        <v>4.6266666666666598</v>
-      </c>
-      <c r="V31" s="1">
-        <v>0.77636194430524696</v>
-      </c>
-    </row>
-    <row r="32" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="Q32">
-        <v>401</v>
-      </c>
-      <c r="R32">
-        <v>245</v>
-      </c>
-      <c r="S32">
-        <v>37.299999999999997</v>
-      </c>
-      <c r="T32">
-        <v>837</v>
-      </c>
-      <c r="U32" s="1">
-        <v>4.2033333333333296</v>
-      </c>
-      <c r="V32" s="1">
-        <v>1.63526629149335</v>
-      </c>
-    </row>
-    <row r="33" spans="17:22" x14ac:dyDescent="0.25">
-      <c r="Q33">
-        <v>342</v>
-      </c>
-      <c r="R33">
-        <v>267</v>
-      </c>
-      <c r="S33">
-        <v>35.200000000000003</v>
-      </c>
-      <c r="T33">
-        <v>734</v>
-      </c>
-      <c r="U33" s="1">
-        <v>5.6866666666666603</v>
-      </c>
-      <c r="V33" s="1">
+      <c r="AB33" s="1">
         <v>1.2822816079047801</v>
       </c>
     </row>
@@ -6396,7 +6575,7 @@
   <dimension ref="A1:DK117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J33"/>
+      <selection activeCell="C1" sqref="C1:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6433,7 +6612,7 @@
         <v>42</v>
       </c>
       <c r="I1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J1" t="s">
         <v>33</v>
@@ -6879,6 +7058,9 @@
       <c r="I15" s="2">
         <v>8.4879038100000006</v>
       </c>
+      <c r="J15" s="2">
+        <v>13.95</v>
+      </c>
       <c r="N15" s="1"/>
     </row>
     <row r="16" spans="1:115" x14ac:dyDescent="0.25">
@@ -7233,7 +7415,9 @@
       <c r="I26" s="2">
         <v>11.83763589</v>
       </c>
-      <c r="J26" s="2"/>
+      <c r="J26" s="2">
+        <v>11.8</v>
+      </c>
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -8166,7 +8350,7 @@
   <dimension ref="A1:U37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I20"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>